<commit_message>
metro buget excercises through question 6
</commit_message>
<xml_diff>
--- a/spreadsheets/metro_budget_exercise.xlsx
+++ b/spreadsheets/metro_budget_exercise.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aimeejohnson/Desktop/DA12/projects/excel-lookups-da12-aimeejohnson/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA87238A-B009-C842-8BDB-20C3B3C78C12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21069C95-9C42-384C-866F-F32C0FC045D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10220" yWindow="860" windowWidth="29360" windowHeight="19460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8360" yWindow="600" windowWidth="33380" windowHeight="19460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metro_budget" sheetId="1" r:id="rId1"/>
     <sheet name="data_dictionary" sheetId="2" r:id="rId2"/>
+    <sheet name="Departments" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -56,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="90">
   <si>
     <t>Department</t>
   </si>
@@ -484,7 +485,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -670,6 +671,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -831,7 +844,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -843,6 +856,8 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1200,8 +1215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F67" sqref="F67"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1228,7 +1243,7 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
@@ -1243,7 +1258,7 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="10" t="s">
         <v>8</v>
       </c>
       <c r="J1" t="s">
@@ -1258,7 +1273,7 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="O1" t="s">
@@ -4429,6 +4444,10 @@
         <f>_xlfn.XLOOKUP(A65,$A$2:$A$52,$I$2:$I$52)</f>
         <v>-27292.159999999974</v>
       </c>
+      <c r="D65">
+        <f>_xlfn.XLOOKUP(A65,$A$2:$A$52,$N$2:$N$52)</f>
+        <v>-9181.0800000000163</v>
+      </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
@@ -4442,6 +4461,10 @@
         <f t="shared" ref="C66:C70" si="10">_xlfn.XLOOKUP(A66,$A$2:$A$52,$I$2:$I$52)</f>
         <v>0</v>
       </c>
+      <c r="D66">
+        <f t="shared" ref="D66:D70" si="11">_xlfn.XLOOKUP(A66,$A$2:$A$52,$N$2:$N$52)</f>
+        <v>-311228.08999999997</v>
+      </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
@@ -4455,6 +4478,10 @@
         <f t="shared" si="10"/>
         <v>-189254.06000000006</v>
       </c>
+      <c r="D67">
+        <f t="shared" si="11"/>
+        <v>-374962.91000000015</v>
+      </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
@@ -4468,6 +4495,10 @@
         <f t="shared" si="10"/>
         <v>-45485.580000000075</v>
       </c>
+      <c r="D68">
+        <f t="shared" si="11"/>
+        <v>-72.879999999888241</v>
+      </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
@@ -4481,6 +4512,10 @@
         <f t="shared" si="10"/>
         <v>-8005.7900000010268</v>
       </c>
+      <c r="D69">
+        <f t="shared" si="11"/>
+        <v>-1724.9000000000233</v>
+      </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
@@ -4494,6 +4529,10 @@
         <f t="shared" si="10"/>
         <v>-133456.33000001032</v>
       </c>
+      <c r="D70">
+        <f t="shared" si="11"/>
+        <v>-82077.349999999627</v>
+      </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="7" t="s">
@@ -4518,31 +4557,103 @@
       <c r="A74" t="s">
         <v>24</v>
       </c>
+      <c r="B74">
+        <f>INDEX($D$2:$D$52,MATCH(A74,$A$2:$A$52,0))</f>
+        <v>-36209.630000000005</v>
+      </c>
+      <c r="C74">
+        <f>INDEX($I$2:$I$52,MATCH(A74,$A$2:$A$52,0))</f>
+        <v>-27292.159999999974</v>
+      </c>
+      <c r="D74">
+        <f>INDEX($N$2:$N$52,MATCH(A74,$A$2:$A$52,0))</f>
+        <v>-9181.0800000000163</v>
+      </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>25</v>
       </c>
+      <c r="B75">
+        <f t="shared" ref="B75:B79" si="12">INDEX($D$2:$D$52,MATCH(A75,$A$2:$A$52,0))</f>
+        <v>0</v>
+      </c>
+      <c r="C75">
+        <f t="shared" ref="C75:C79" si="13">INDEX($I$2:$I$52,MATCH(A75,$A$2:$A$52,0))</f>
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <f t="shared" ref="D75:D79" si="14">INDEX($N$2:$N$52,MATCH(A75,$A$2:$A$52,0))</f>
+        <v>-311228.08999999997</v>
+      </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>32</v>
       </c>
+      <c r="B76">
+        <f t="shared" si="12"/>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="13"/>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="14"/>
+        <v>-374962.91000000015</v>
+      </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>38</v>
       </c>
+      <c r="B77">
+        <f t="shared" si="12"/>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="C77">
+        <f t="shared" si="13"/>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="14"/>
+        <v>-72.879999999888241</v>
+      </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>39</v>
       </c>
+      <c r="B78">
+        <f t="shared" si="12"/>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="C78">
+        <f t="shared" si="13"/>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="14"/>
+        <v>-1724.9000000000233</v>
+      </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>55</v>
       </c>
+      <c r="B79">
+        <f t="shared" si="12"/>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="C79">
+        <f t="shared" si="13"/>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="D79">
+        <f t="shared" si="14"/>
+        <v>-82077.349999999627</v>
+      </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="7" t="s">
@@ -4553,6 +4664,9 @@
       <c r="A82" t="s">
         <v>0</v>
       </c>
+      <c r="B82" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B83" s="1" t="s">
@@ -4566,22 +4680,40 @@
       <c r="A84" t="s">
         <v>73</v>
       </c>
-      <c r="B84" s="6"/>
-      <c r="C84" s="6"/>
+      <c r="B84" s="6">
+        <f>INDEX($B$2:$B$52,MATCH(B82,$A$2:$A$52,0))</f>
+        <v>356640100</v>
+      </c>
+      <c r="C84" s="6">
+        <f>INDEX($C$2:$C$52,MATCH(B82,$A$2:$A$52,0))</f>
+        <v>341243679.13</v>
+      </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>74</v>
       </c>
-      <c r="B85" s="6"/>
-      <c r="C85" s="6"/>
+      <c r="B85" s="6">
+        <f>INDEX($G$2:$G$52,MATCH(B82,$A$2:$A$52,0))</f>
+        <v>382685200</v>
+      </c>
+      <c r="C85" s="6">
+        <f>INDEX($H$2:$H$52,MATCH(B82,$A$2:$A$52,0))</f>
+        <v>346340810.81999999</v>
+      </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>75</v>
       </c>
-      <c r="B86" s="6"/>
-      <c r="C86" s="6"/>
+      <c r="B86" s="6">
+        <f>INDEX($L$2:$L$52,MATCH(B82,$A$2:$A$52,0))</f>
+        <v>376548600</v>
+      </c>
+      <c r="C86" s="6">
+        <f>INDEX($M$2:$M$52,MATCH(B82,$A$2:$A$524,0))</f>
+        <v>355279492.22999901</v>
+      </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
@@ -4718,10 +4850,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A83" xr:uid="{0ECE0BAD-DC74-4E7B-8842-0609702F3664}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A83 B82" xr:uid="{0ECE0BAD-DC74-4E7B-8842-0609702F3664}">
       <formula1>$A$2:$A$52</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B82:B83" xr:uid="{1248789C-8354-428B-8B98-C97B02054C67}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B83" xr:uid="{1248789C-8354-428B-8B98-C97B02054C67}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4824,4 +4956,274 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52752DFF-A038-4B47-868F-46CE0C158B4F}">
+  <dimension ref="A1:A51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
metro budget exercise working on question 7
</commit_message>
<xml_diff>
--- a/spreadsheets/metro_budget_exercise.xlsx
+++ b/spreadsheets/metro_budget_exercise.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aimeejohnson/Desktop/DA12/projects/excel-lookups-da12-aimeejohnson/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21069C95-9C42-384C-866F-F32C0FC045D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C2012A-A2B3-1349-B35A-C93BA474F3C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8360" yWindow="600" windowWidth="33380" windowHeight="19460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2960" yWindow="500" windowWidth="34040" windowHeight="20320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metro_budget" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="91">
   <si>
     <t>Department</t>
   </si>
@@ -327,6 +327,9 @@
   </si>
   <si>
     <t>Actual spending amount - budget amount for fiscal year 2019</t>
+  </si>
+  <si>
+    <t>Question 7</t>
   </si>
 </sst>
 </file>
@@ -337,7 +340,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -484,8 +487,15 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -683,6 +693,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -844,7 +860,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -858,6 +874,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1215,8 +1235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="G74" sqref="G74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1224,7 +1244,7 @@
     <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="26.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.83203125" customWidth="1"/>
-    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.6640625" customWidth="1"/>
     <col min="7" max="7" width="15.5" customWidth="1"/>
     <col min="8" max="8" width="26.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="12" width="15.83203125" customWidth="1"/>
@@ -1234,52 +1254,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="10" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="14" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1287,21 +1307,21 @@
       <c r="A2" t="s">
         <v>16</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="12">
         <v>356640100</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="12">
         <v>341243679.13</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="12">
         <f>C2-B2</f>
         <v>-15396420.870000005</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="13">
         <f>IFERROR(D2/B2,0)</f>
         <v>-4.3170750765267295E-2</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="12">
         <f>RANK(E2,E:E,0)</f>
         <v>38</v>
       </c>
@@ -1346,21 +1366,21 @@
       <c r="A3" t="s">
         <v>17</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="12">
         <v>328800</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="12">
         <v>321214.59000000003</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="12">
         <f t="shared" ref="D3:D52" si="0">C3-B3</f>
         <v>-7585.4099999999744</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="13">
         <f t="shared" ref="E3:E52" si="1">IFERROR(D3/B3,0)</f>
         <v>-2.3069981751824741E-2</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="12">
         <f t="shared" ref="F3:F52" si="2">RANK(E3,E:E,0)</f>
         <v>30</v>
       </c>
@@ -1405,21 +1425,21 @@
       <c r="A4" t="s">
         <v>18</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="12">
         <v>3130600</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="12">
         <v>3115157.5599999898</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="12">
         <f t="shared" si="0"/>
         <v>-15442.440000010189</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="13">
         <f t="shared" si="1"/>
         <v>-4.9327413275443007E-3</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="12">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
@@ -1464,21 +1484,21 @@
       <c r="A5" t="s">
         <v>19</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="12">
         <v>7670700</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="12">
         <v>6947552.6699999999</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="12">
         <f t="shared" si="0"/>
         <v>-723147.33000000007</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="13">
         <f t="shared" si="1"/>
         <v>-9.4273968477453174E-2</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="12">
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
@@ -1523,21 +1543,21 @@
       <c r="A6" t="s">
         <v>20</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="12">
         <v>409300</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="12">
         <v>385908.52</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="12">
         <f t="shared" si="0"/>
         <v>-23391.479999999981</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="13">
         <f t="shared" si="1"/>
         <v>-5.7149963352064452E-2</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="12">
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
@@ -1582,21 +1602,21 @@
       <c r="A7" t="s">
         <v>21</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="12">
         <v>3329000</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="12">
         <v>2946071.21</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="12">
         <f t="shared" si="0"/>
         <v>-382928.79000000004</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="13">
         <f t="shared" si="1"/>
         <v>-0.11502817362571344</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="12">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
@@ -1641,21 +1661,21 @@
       <c r="A8" t="s">
         <v>22</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="12">
         <v>1552100</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="12">
         <v>1315623.30999999</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="12">
         <f t="shared" si="0"/>
         <v>-236476.69000000996</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="13">
         <f t="shared" si="1"/>
         <v>-0.15235918433091292</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="12">
         <f t="shared" si="2"/>
         <v>51</v>
       </c>
@@ -1700,21 +1720,21 @@
       <c r="A9" t="s">
         <v>23</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="12">
         <v>9349400</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="12">
         <v>8952825.2799999993</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="12">
         <f t="shared" si="0"/>
         <v>-396574.72000000067</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="13">
         <f t="shared" si="1"/>
         <v>-4.2417130511048909E-2</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="12">
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
@@ -1759,21 +1779,21 @@
       <c r="A10" t="s">
         <v>24</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="12">
         <v>443300</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="12">
         <v>407090.37</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="12">
         <f t="shared" si="0"/>
         <v>-36209.630000000005</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="13">
         <f t="shared" si="1"/>
         <v>-8.1681998646514792E-2</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="12">
         <f t="shared" si="2"/>
         <v>46</v>
       </c>
@@ -1818,21 +1838,21 @@
       <c r="A11" t="s">
         <v>25</v>
       </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
+      <c r="B11" s="12">
+        <v>0</v>
+      </c>
+      <c r="C11" s="12">
+        <v>0</v>
+      </c>
+      <c r="D11" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="12">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
@@ -1877,21 +1897,21 @@
       <c r="A12" t="s">
         <v>26</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="12">
         <v>4280900</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="12">
         <v>4066595.33</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="12">
         <f t="shared" si="0"/>
         <v>-214304.66999999993</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="13">
         <f t="shared" si="1"/>
         <v>-5.0060657805601608E-2</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="12">
         <f t="shared" si="2"/>
         <v>39</v>
       </c>
@@ -1936,21 +1956,21 @@
       <c r="A13" t="s">
         <v>27</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="12">
         <v>5847800</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="12">
         <v>5772288.3300000001</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="12">
         <f t="shared" si="0"/>
         <v>-75511.669999999925</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="13">
         <f t="shared" si="1"/>
         <v>-1.2912833886247806E-2</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="12">
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
@@ -1995,21 +2015,21 @@
       <c r="A14" t="s">
         <v>28</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="12">
         <v>512000</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="12">
         <v>505017.37</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="12">
         <f t="shared" si="0"/>
         <v>-6982.6300000000047</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="13">
         <f t="shared" si="1"/>
         <v>-1.3637949218750009E-2</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="12">
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
@@ -2054,21 +2074,21 @@
       <c r="A15" t="s">
         <v>29</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="12">
         <v>156049100</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="12">
         <v>156545919.90000001</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="12">
         <f t="shared" si="0"/>
         <v>496819.90000000596</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="13">
         <f t="shared" si="1"/>
         <v>3.1837408866824991E-3</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="12">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -2113,21 +2133,21 @@
       <c r="A16" t="s">
         <v>30</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="12">
         <v>6600700</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="12">
         <v>6522480.4599999897</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="12">
         <f t="shared" si="0"/>
         <v>-78219.540000010282</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="13">
         <f t="shared" si="1"/>
         <v>-1.1850188616360429E-2</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="12">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
@@ -2172,21 +2192,21 @@
       <c r="A17" t="s">
         <v>31</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="12">
         <v>14860800</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="12">
         <v>14439480.050000001</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="12">
         <f t="shared" si="0"/>
         <v>-421319.94999999925</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="13">
         <f t="shared" si="1"/>
         <v>-2.8351094826658003E-2</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="12">
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
@@ -2231,21 +2251,21 @@
       <c r="A18" t="s">
         <v>32</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="12">
         <v>2764700</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="12">
         <v>2615303.8999999901</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="12">
         <f t="shared" si="0"/>
         <v>-149396.10000000987</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="13">
         <f t="shared" si="1"/>
         <v>-5.4037002206391245E-2</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="12">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
@@ -2290,21 +2310,21 @@
       <c r="A19" t="s">
         <v>33</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="12">
         <v>8837300</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="12">
         <v>8460963.1999999899</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="12">
         <f t="shared" si="0"/>
         <v>-376336.80000001006</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="13">
         <f t="shared" si="1"/>
         <v>-4.258504294298146E-2</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="12">
         <f t="shared" si="2"/>
         <v>37</v>
       </c>
@@ -2349,21 +2369,21 @@
       <c r="A20" t="s">
         <v>34</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="12">
         <v>124385900</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="12">
         <v>124384360.159999</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="12">
         <f t="shared" si="0"/>
         <v>-1539.8400010019541</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="13">
         <f t="shared" si="1"/>
         <v>-1.2379538203300809E-5</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="12">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
@@ -2408,21 +2428,21 @@
       <c r="A21" t="s">
         <v>35</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="12">
         <v>24332100</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="12">
         <v>22408587.5499999</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="12">
         <f t="shared" si="0"/>
         <v>-1923512.4500000998</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="13">
         <f t="shared" si="1"/>
         <v>-7.9052463618023094E-2</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="12">
         <f t="shared" si="2"/>
         <v>43</v>
       </c>
@@ -2467,21 +2487,21 @@
       <c r="A22" t="s">
         <v>36</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="12">
         <v>11566000</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="12">
         <v>11412339.8799999</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="12">
         <f t="shared" si="0"/>
         <v>-153660.12000009976</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="13">
         <f t="shared" si="1"/>
         <v>-1.3285502334437123E-2</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="12">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
@@ -2526,21 +2546,21 @@
       <c r="A23" t="s">
         <v>37</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="12">
         <v>20862700</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="12">
         <v>20036743.4099999</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="12">
         <f t="shared" si="0"/>
         <v>-825956.59000010043</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="13">
         <f t="shared" si="1"/>
         <v>-3.9590110100806722E-2</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="12">
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
@@ -2585,21 +2605,21 @@
       <c r="A24" t="s">
         <v>38</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="12">
         <v>917200</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="12">
         <v>904969.19</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="12">
         <f t="shared" si="0"/>
         <v>-12230.810000000056</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="13">
         <f t="shared" si="1"/>
         <v>-1.3334943305713101E-2</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="12">
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
@@ -2644,21 +2664,21 @@
       <c r="A25" t="s">
         <v>39</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="12">
         <v>484100</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="12">
         <v>479149.53</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="12">
         <f t="shared" si="0"/>
         <v>-4950.4699999999721</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25" s="13">
         <f t="shared" si="1"/>
         <v>-1.0226130964676661E-2</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="12">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
@@ -2703,21 +2723,21 @@
       <c r="A26" t="s">
         <v>40</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="12">
         <v>5249800</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="12">
         <v>4801960.08</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="12">
         <f t="shared" si="0"/>
         <v>-447839.91999999993</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E26" s="13">
         <f t="shared" si="1"/>
         <v>-8.5306091660634673E-2</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="12">
         <f t="shared" si="2"/>
         <v>47</v>
       </c>
@@ -2762,21 +2782,21 @@
       <c r="A27" t="s">
         <v>41</v>
       </c>
-      <c r="B27">
-        <v>0</v>
-      </c>
-      <c r="C27">
-        <v>0</v>
-      </c>
-      <c r="D27">
+      <c r="B27" s="12">
+        <v>0</v>
+      </c>
+      <c r="C27" s="12">
+        <v>0</v>
+      </c>
+      <c r="D27" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E27" s="5">
+      <c r="E27" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="12">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
@@ -2821,21 +2841,21 @@
       <c r="A28" t="s">
         <v>42</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="12">
         <v>1382900</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="12">
         <v>1250442.02</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="12">
         <f t="shared" si="0"/>
         <v>-132457.97999999998</v>
       </c>
-      <c r="E28" s="5">
+      <c r="E28" s="13">
         <f t="shared" si="1"/>
         <v>-9.5782760864849215E-2</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="12">
         <f t="shared" si="2"/>
         <v>49</v>
       </c>
@@ -2880,21 +2900,21 @@
       <c r="A29" t="s">
         <v>43</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="12">
         <v>2561800</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="12">
         <v>2523884.71</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="12">
         <f t="shared" si="0"/>
         <v>-37915.290000000037</v>
       </c>
-      <c r="E29" s="5">
+      <c r="E29" s="13">
         <f t="shared" si="1"/>
         <v>-1.4800253727847622E-2</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="12">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
@@ -2939,21 +2959,21 @@
       <c r="A30" t="s">
         <v>44</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="12">
         <v>12132200</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="12">
         <v>12030494.1</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="12">
         <f t="shared" si="0"/>
         <v>-101705.90000000037</v>
       </c>
-      <c r="E30" s="5">
+      <c r="E30" s="13">
         <f t="shared" si="1"/>
         <v>-8.3831374359143746E-3</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="12">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
@@ -2998,21 +3018,21 @@
       <c r="A31" t="s">
         <v>45</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="12">
         <v>1765600</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="12">
         <v>1740827.69</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="12">
         <f t="shared" si="0"/>
         <v>-24772.310000000056</v>
       </c>
-      <c r="E31" s="5">
+      <c r="E31" s="13">
         <f t="shared" si="1"/>
         <v>-1.4030533529678329E-2</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="12">
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
@@ -3057,21 +3077,21 @@
       <c r="A32" t="s">
         <v>46</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="12">
         <v>5999400</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="12">
         <v>5925637.7199999904</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="12">
         <f t="shared" si="0"/>
         <v>-73762.280000009574</v>
       </c>
-      <c r="E32" s="5">
+      <c r="E32" s="13">
         <f t="shared" si="1"/>
         <v>-1.2294942827617691E-2</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="12">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
@@ -3116,21 +3136,21 @@
       <c r="A33" t="s">
         <v>47</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="12">
         <v>927703099.99999905</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="12">
         <v>920284264.73000002</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="12">
         <f t="shared" si="0"/>
         <v>-7418835.2699990273</v>
       </c>
-      <c r="E33" s="5">
+      <c r="E33" s="13">
         <f t="shared" si="1"/>
         <v>-7.9969930789269058E-3</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="12">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
@@ -3175,21 +3195,21 @@
       <c r="A34" t="s">
         <v>48</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="12">
         <v>4189300</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="12">
         <v>4109958.22</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="12">
         <f t="shared" si="0"/>
         <v>-79341.779999999795</v>
       </c>
-      <c r="E34" s="5">
+      <c r="E34" s="13">
         <f t="shared" si="1"/>
         <v>-1.8939149738619768E-2</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="12">
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
@@ -3234,21 +3254,21 @@
       <c r="A35" t="s">
         <v>49</v>
       </c>
-      <c r="B35">
-        <v>0</v>
-      </c>
-      <c r="C35">
-        <v>0</v>
-      </c>
-      <c r="D35">
+      <c r="B35" s="12">
+        <v>0</v>
+      </c>
+      <c r="C35" s="12">
+        <v>0</v>
+      </c>
+      <c r="D35" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E35" s="5">
+      <c r="E35" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="12">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
@@ -3293,21 +3313,21 @@
       <c r="A36" t="s">
         <v>50</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="12">
         <v>798200</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="12">
         <v>735423.27999999898</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="12">
         <f t="shared" si="0"/>
         <v>-62776.72000000102</v>
       </c>
-      <c r="E36" s="5">
+      <c r="E36" s="13">
         <f t="shared" si="1"/>
         <v>-7.8647857679780775E-2</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="12">
         <f t="shared" si="2"/>
         <v>42</v>
       </c>
@@ -3352,21 +3372,21 @@
       <c r="A37" t="s">
         <v>51</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="12">
         <v>2087800</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="12">
         <v>2005447.73999999</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="12">
         <f t="shared" si="0"/>
         <v>-82352.260000010021</v>
       </c>
-      <c r="E37" s="5">
+      <c r="E37" s="13">
         <f t="shared" si="1"/>
         <v>-3.9444515758219188E-2</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="12">
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
@@ -3411,21 +3431,21 @@
       <c r="A38" t="s">
         <v>52</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="12">
         <v>855300</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="12">
         <v>838669.82</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="12">
         <f t="shared" si="0"/>
         <v>-16630.180000000051</v>
       </c>
-      <c r="E38" s="5">
+      <c r="E38" s="13">
         <f t="shared" si="1"/>
         <v>-1.9443680579913542E-2</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="12">
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
@@ -3470,21 +3490,21 @@
       <c r="A39" t="s">
         <v>53</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="12">
         <v>883900</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="12">
         <v>813108.87</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="12">
         <f t="shared" si="0"/>
         <v>-70791.13</v>
       </c>
-      <c r="E39" s="5">
+      <c r="E39" s="13">
         <f t="shared" si="1"/>
         <v>-8.008952370177623E-2</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="12">
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
@@ -3529,21 +3549,21 @@
       <c r="A40" t="s">
         <v>54</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="12">
         <v>38381900</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="12">
         <v>37565141.859999903</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="12">
         <f t="shared" si="0"/>
         <v>-816758.14000009745</v>
       </c>
-      <c r="E40" s="5">
+      <c r="E40" s="13">
         <f t="shared" si="1"/>
         <v>-2.1279773539092578E-2</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="12">
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
@@ -3588,21 +3608,21 @@
       <c r="A41" t="s">
         <v>55</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="12">
         <v>4593300</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="12">
         <v>4409060.2099999897</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="12">
         <f t="shared" si="0"/>
         <v>-184239.79000001028</v>
       </c>
-      <c r="E41" s="5">
+      <c r="E41" s="13">
         <f t="shared" si="1"/>
         <v>-4.0110550149132493E-2</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="12">
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
@@ -3647,21 +3667,21 @@
       <c r="A42" t="s">
         <v>56</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="12">
         <v>188593300</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="12">
         <v>188551675.67999899</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="12">
         <f t="shared" si="0"/>
         <v>-41624.320001006126</v>
       </c>
-      <c r="E42" s="5">
+      <c r="E42" s="13">
         <f t="shared" si="1"/>
         <v>-2.2070943135841053E-4</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="12">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
@@ -3706,21 +3726,21 @@
       <c r="A43" t="s">
         <v>57</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="12">
         <v>8135400</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="12">
         <v>7968645.8300000001</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="12">
         <f t="shared" si="0"/>
         <v>-166754.16999999993</v>
       </c>
-      <c r="E43" s="5">
+      <c r="E43" s="13">
         <f t="shared" si="1"/>
         <v>-2.0497353541313264E-2</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="12">
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
@@ -3765,21 +3785,21 @@
       <c r="A44" t="s">
         <v>58</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="12">
         <v>30083200</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="12">
         <v>29789104.379999999</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="12">
         <f t="shared" si="0"/>
         <v>-294095.62000000104</v>
       </c>
-      <c r="E44" s="5">
+      <c r="E44" s="13">
         <f t="shared" si="1"/>
         <v>-9.7760750186150751E-3</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="12">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
@@ -3824,21 +3844,21 @@
       <c r="A45" t="s">
         <v>59</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="12">
         <v>55301600</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="12">
         <v>54589584.0499999</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="12">
         <f t="shared" si="0"/>
         <v>-712015.95000009984</v>
       </c>
-      <c r="E45" s="5">
+      <c r="E45" s="13">
         <f t="shared" si="1"/>
         <v>-1.287514194887851E-2</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="12">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
@@ -3883,21 +3903,21 @@
       <c r="A46" t="s">
         <v>60</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="12">
         <v>259100</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="12">
         <v>258322.43</v>
       </c>
-      <c r="D46">
+      <c r="D46" s="12">
         <f t="shared" si="0"/>
         <v>-777.57000000000698</v>
       </c>
-      <c r="E46" s="5">
+      <c r="E46" s="13">
         <f t="shared" si="1"/>
         <v>-3.0010420686993711E-3</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="12">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
@@ -3942,21 +3962,21 @@
       <c r="A47" t="s">
         <v>61</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="12">
         <v>70390700</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="12">
         <v>70378426.719999999</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="12">
         <f t="shared" si="0"/>
         <v>-12273.280000001192</v>
       </c>
-      <c r="E47" s="5">
+      <c r="E47" s="13">
         <f t="shared" si="1"/>
         <v>-1.7435939690898361E-4</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="12">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
@@ -4001,21 +4021,21 @@
       <c r="A48" t="s">
         <v>62</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="12">
         <v>6737100</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="12">
         <v>6527352.5699999901</v>
       </c>
-      <c r="D48">
+      <c r="D48" s="12">
         <f t="shared" si="0"/>
         <v>-209747.43000000995</v>
       </c>
-      <c r="E48" s="5">
+      <c r="E48" s="13">
         <f t="shared" si="1"/>
         <v>-3.1133192323107857E-2</v>
       </c>
-      <c r="F48">
+      <c r="F48" s="12">
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
@@ -4060,21 +4080,21 @@
       <c r="A49" t="s">
         <v>63</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="12">
         <v>92200</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="12">
         <v>90499.43</v>
       </c>
-      <c r="D49">
+      <c r="D49" s="12">
         <f t="shared" si="0"/>
         <v>-1700.570000000007</v>
       </c>
-      <c r="E49" s="5">
+      <c r="E49" s="13">
         <f t="shared" si="1"/>
         <v>-1.8444360086767971E-2</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="12">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
@@ -4119,21 +4139,21 @@
       <c r="A50" t="s">
         <v>64</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="12">
         <v>832600</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="12">
         <v>832600</v>
       </c>
-      <c r="D50">
+      <c r="D50" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E50" s="5">
+      <c r="E50" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F50">
+      <c r="F50" s="12">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
@@ -4178,21 +4198,21 @@
       <c r="A51" t="s">
         <v>65</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="12">
         <v>8609500</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="12">
         <v>8499425.3399999905</v>
       </c>
-      <c r="D51">
+      <c r="D51" s="12">
         <f t="shared" si="0"/>
         <v>-110074.66000000946</v>
       </c>
-      <c r="E51" s="5">
+      <c r="E51" s="13">
         <f t="shared" si="1"/>
         <v>-1.2785255822058129E-2</v>
       </c>
-      <c r="F51">
+      <c r="F51" s="12">
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
@@ -4237,21 +4257,21 @@
       <c r="A52" t="s">
         <v>66</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="12">
         <v>2451000</v>
       </c>
-      <c r="C52">
+      <c r="C52" s="12">
         <v>2254684.7999999998</v>
       </c>
-      <c r="D52">
+      <c r="D52" s="12">
         <f t="shared" si="0"/>
         <v>-196315.20000000019</v>
       </c>
-      <c r="E52" s="5">
+      <c r="E52" s="13">
         <f t="shared" si="1"/>
         <v>-8.009596083231342E-2</v>
       </c>
-      <c r="F52">
+      <c r="F52" s="12">
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
@@ -4296,6 +4316,9 @@
       <c r="A54" s="2" t="s">
         <v>67</v>
       </c>
+      <c r="F54" s="11" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
@@ -4308,6 +4331,18 @@
         <v>8</v>
       </c>
       <c r="D55" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I55" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -4327,6 +4362,21 @@
         <f t="array" ref="D56">VLOOKUP(A56,$A$1:$P$52,COLUMN(N:N),FALSE)</f>
         <v>-9181.0800000000163</v>
       </c>
+      <c r="F56" t="s">
+        <v>24</v>
+      </c>
+      <c r="G56">
+        <f>VLOOKUP($F56,$A$1:$P$52,MATCH($G$55,$A$1:$P$1),FALSE)</f>
+        <v>-36209.630000000005</v>
+      </c>
+      <c r="H56">
+        <f t="shared" ref="H56:I61" si="9">VLOOKUP($F56,$A$1:$P$52,MATCH($G$55,$A$1:$P$1),FALSE)</f>
+        <v>-36209.630000000005</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="9"/>
+        <v>-36209.630000000005</v>
+      </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
@@ -4344,6 +4394,21 @@
         <f t="array" ref="D57">VLOOKUP(A57,$A$1:$P$52,COLUMN(N:N),FALSE)</f>
         <v>-311228.08999999997</v>
       </c>
+      <c r="F57" t="s">
+        <v>25</v>
+      </c>
+      <c r="G57">
+        <f t="shared" ref="G57:G61" si="10">VLOOKUP($F57,$A$1:$P$52,MATCH($G$55,$A$1:$P$1),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
@@ -4361,6 +4426,21 @@
         <f t="array" ref="D58">VLOOKUP(A58,$A$1:$P$52,COLUMN(N:N),FALSE)</f>
         <v>-374962.91000000015</v>
       </c>
+      <c r="F58" t="s">
+        <v>32</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="10"/>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="H58">
+        <f t="shared" si="9"/>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="I58">
+        <f t="shared" si="9"/>
+        <v>-149396.10000000987</v>
+      </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
@@ -4378,6 +4458,21 @@
         <f t="array" ref="D59">VLOOKUP(A59,$A$1:$P$52,COLUMN(N:N),FALSE)</f>
         <v>-72.879999999888241</v>
       </c>
+      <c r="F59" t="s">
+        <v>38</v>
+      </c>
+      <c r="G59">
+        <f t="shared" si="10"/>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="H59">
+        <f t="shared" si="9"/>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="I59">
+        <f t="shared" si="9"/>
+        <v>-12230.810000000056</v>
+      </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
@@ -4395,6 +4490,21 @@
         <f t="array" ref="D60">VLOOKUP(A60,$A$1:$P$52,COLUMN(N:N),FALSE)</f>
         <v>-1724.9000000000233</v>
       </c>
+      <c r="F60" t="s">
+        <v>39</v>
+      </c>
+      <c r="G60">
+        <f t="shared" si="10"/>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="H60">
+        <f t="shared" si="9"/>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="I60">
+        <f t="shared" si="9"/>
+        <v>-4950.4699999999721</v>
+      </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
@@ -4412,11 +4522,27 @@
         <f t="array" ref="D61">VLOOKUP(A61,$A$1:$P$52,COLUMN(N:N),FALSE)</f>
         <v>-82077.349999999627</v>
       </c>
+      <c r="F61" t="s">
+        <v>55</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="10"/>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="H61">
+        <f t="shared" si="9"/>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="9"/>
+        <v>-184239.79000001028</v>
+      </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A63" s="7" t="s">
         <v>68</v>
       </c>
+      <c r="F63" s="7"/>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
@@ -4431,8 +4557,20 @@
       <c r="D64" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>24</v>
       </c>
@@ -4448,98 +4586,189 @@
         <f>_xlfn.XLOOKUP(A65,$A$2:$A$52,$N$2:$N$52)</f>
         <v>-9181.0800000000163</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F65" t="s">
+        <v>24</v>
+      </c>
+      <c r="G65" t="e">
+        <f>_xlfn.XLOOKUP(F65,$A$2:$A$52,MATCH(G64,$A$1:$P$1,0))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H65">
+        <f>_xlfn.XLOOKUP(F65,$A$2:$A$52,$I$2:$I$52)</f>
+        <v>-27292.159999999974</v>
+      </c>
+      <c r="I65">
+        <f>_xlfn.XLOOKUP(F65,$A$2:$A$52,$N$2:$N$52)</f>
+        <v>-9181.0800000000163</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>25</v>
       </c>
       <c r="B66">
-        <f t="shared" ref="B66:B70" si="9">_xlfn.XLOOKUP(A66,$A$2:$A$52,$D$2:$D$52)</f>
+        <f t="shared" ref="B66:B70" si="11">_xlfn.XLOOKUP(A66,$A$2:$A$52,$D$2:$D$52)</f>
         <v>0</v>
       </c>
       <c r="C66">
-        <f t="shared" ref="C66:C70" si="10">_xlfn.XLOOKUP(A66,$A$2:$A$52,$I$2:$I$52)</f>
+        <f t="shared" ref="C66:C70" si="12">_xlfn.XLOOKUP(A66,$A$2:$A$52,$I$2:$I$52)</f>
         <v>0</v>
       </c>
       <c r="D66">
-        <f t="shared" ref="D66:D70" si="11">_xlfn.XLOOKUP(A66,$A$2:$A$52,$N$2:$N$52)</f>
+        <f t="shared" ref="D66:D70" si="13">_xlfn.XLOOKUP(A66,$A$2:$A$52,$N$2:$N$52)</f>
         <v>-311228.08999999997</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F66" t="s">
+        <v>25</v>
+      </c>
+      <c r="G66">
+        <f>_xlfn.XLOOKUP(F66,$A$2:$A$52,$D$2:$D$52)</f>
+        <v>0</v>
+      </c>
+      <c r="H66">
+        <f t="shared" ref="H66:H70" si="14">_xlfn.XLOOKUP(F66,$A$2:$A$52,$I$2:$I$52)</f>
+        <v>0</v>
+      </c>
+      <c r="I66">
+        <f t="shared" ref="I66:I70" si="15">_xlfn.XLOOKUP(F66,$A$2:$A$52,$N$2:$N$52)</f>
+        <v>-311228.08999999997</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>32</v>
       </c>
       <c r="B67">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-149396.10000000987</v>
       </c>
       <c r="C67">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="D67">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-374962.91000000015</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F67" t="s">
+        <v>32</v>
+      </c>
+      <c r="G67">
+        <f t="shared" ref="G66:G70" si="16">_xlfn.XLOOKUP(F67,$A$2:$A$52,$D$2:$D$52)</f>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="H67">
+        <f t="shared" si="14"/>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="I67">
+        <f t="shared" si="15"/>
+        <v>-374962.91000000015</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>38</v>
       </c>
       <c r="B68">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-12230.810000000056</v>
       </c>
       <c r="C68">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="D68">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-72.879999999888241</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F68" t="s">
+        <v>38</v>
+      </c>
+      <c r="G68">
+        <f t="shared" si="16"/>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="H68">
+        <f t="shared" si="14"/>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="I68">
+        <f t="shared" si="15"/>
+        <v>-72.879999999888241</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>39</v>
       </c>
       <c r="B69">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-4950.4699999999721</v>
       </c>
       <c r="C69">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D69">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-1724.9000000000233</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F69" t="s">
+        <v>39</v>
+      </c>
+      <c r="G69">
+        <f t="shared" si="16"/>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="H69">
+        <f t="shared" si="14"/>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="I69">
+        <f t="shared" si="15"/>
+        <v>-1724.9000000000233</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>55</v>
       </c>
       <c r="B70">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-184239.79000001028</v>
       </c>
       <c r="C70">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="D70">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-82077.349999999627</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F70" t="s">
+        <v>55</v>
+      </c>
+      <c r="G70">
+        <f t="shared" si="16"/>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="H70">
+        <f t="shared" si="14"/>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="I70">
+        <f t="shared" si="15"/>
+        <v>-82077.349999999627</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="7" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F72" s="7"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>0</v>
       </c>
@@ -4552,8 +4781,20 @@
       <c r="D73" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F73" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I73" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>24</v>
       </c>
@@ -4569,89 +4810,179 @@
         <f>INDEX($N$2:$N$52,MATCH(A74,$A$2:$A$52,0))</f>
         <v>-9181.0800000000163</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F74" t="s">
+        <v>24</v>
+      </c>
+      <c r="G74" t="e">
+        <f>INDEX($D$2:$D$52,MATCH(F74,$A$2:$A$52,0),MATCH(G73,$A$1:$P$1,0))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="H74">
+        <f>INDEX($I$2:$I$52,MATCH(F74,$A$2:$A$52,0))</f>
+        <v>-27292.159999999974</v>
+      </c>
+      <c r="I74">
+        <f>INDEX($N$2:$N$52,MATCH(F74,$A$2:$A$52,0))</f>
+        <v>-9181.0800000000163</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>25</v>
       </c>
       <c r="B75">
-        <f t="shared" ref="B75:B79" si="12">INDEX($D$2:$D$52,MATCH(A75,$A$2:$A$52,0))</f>
+        <f t="shared" ref="B75:B79" si="17">INDEX($D$2:$D$52,MATCH(A75,$A$2:$A$52,0))</f>
         <v>0</v>
       </c>
       <c r="C75">
-        <f t="shared" ref="C75:C79" si="13">INDEX($I$2:$I$52,MATCH(A75,$A$2:$A$52,0))</f>
+        <f t="shared" ref="C75:C79" si="18">INDEX($I$2:$I$52,MATCH(A75,$A$2:$A$52,0))</f>
         <v>0</v>
       </c>
       <c r="D75">
-        <f t="shared" ref="D75:D79" si="14">INDEX($N$2:$N$52,MATCH(A75,$A$2:$A$52,0))</f>
+        <f t="shared" ref="D75:D79" si="19">INDEX($N$2:$N$52,MATCH(A75,$A$2:$A$52,0))</f>
         <v>-311228.08999999997</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F75" t="s">
+        <v>25</v>
+      </c>
+      <c r="G75">
+        <f t="shared" ref="G75:G79" si="20">INDEX($D$2:$D$52,MATCH(F75,$A$2:$A$52,0))</f>
+        <v>0</v>
+      </c>
+      <c r="H75">
+        <f t="shared" ref="H75:H79" si="21">INDEX($I$2:$I$52,MATCH(F75,$A$2:$A$52,0))</f>
+        <v>0</v>
+      </c>
+      <c r="I75">
+        <f t="shared" ref="I75:I79" si="22">INDEX($N$2:$N$52,MATCH(F75,$A$2:$A$52,0))</f>
+        <v>-311228.08999999997</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>32</v>
       </c>
       <c r="B76">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>-149396.10000000987</v>
       </c>
       <c r="C76">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="D76">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>-374962.91000000015</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F76" t="s">
+        <v>32</v>
+      </c>
+      <c r="G76">
+        <f t="shared" si="20"/>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="H76">
+        <f t="shared" si="21"/>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="I76">
+        <f t="shared" si="22"/>
+        <v>-374962.91000000015</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>38</v>
       </c>
       <c r="B77">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>-12230.810000000056</v>
       </c>
       <c r="C77">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="D77">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>-72.879999999888241</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F77" t="s">
+        <v>38</v>
+      </c>
+      <c r="G77">
+        <f t="shared" si="20"/>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="H77">
+        <f t="shared" si="21"/>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="I77">
+        <f t="shared" si="22"/>
+        <v>-72.879999999888241</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>39</v>
       </c>
       <c r="B78">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>-4950.4699999999721</v>
       </c>
       <c r="C78">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D78">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
         <v>-1724.9000000000233</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F78" t="s">
+        <v>39</v>
+      </c>
+      <c r="G78">
+        <f t="shared" si="20"/>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="H78">
+        <f t="shared" si="21"/>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="I78">
+        <f t="shared" si="22"/>
+        <v>-1724.9000000000233</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>55</v>
       </c>
       <c r="B79">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>-184239.79000001028</v>
       </c>
       <c r="C79">
-        <f t="shared" si="13"/>
+        <f t="shared" si="18"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="D79">
-        <f t="shared" si="14"/>
+        <f t="shared" si="19"/>
+        <v>-82077.349999999627</v>
+      </c>
+      <c r="F79" t="s">
+        <v>55</v>
+      </c>
+      <c r="G79">
+        <f t="shared" si="20"/>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="H79">
+        <f t="shared" si="21"/>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="I79">
+        <f t="shared" si="22"/>
         <v>-82077.349999999627</v>
       </c>
     </row>

</xml_diff>

<commit_message>
metro budget exercises through question 9
</commit_message>
<xml_diff>
--- a/spreadsheets/metro_budget_exercise.xlsx
+++ b/spreadsheets/metro_budget_exercise.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aimeejohnson/Desktop/DA12/projects/excel-lookups-da12-aimeejohnson/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aimeejohnson/Desktop/DA12/projects/excel-lookups-da12-aimeejohnson/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C2012A-A2B3-1349-B35A-C93BA474F3C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04AE6114-9129-BD44-B833-5ADC6572A845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2960" yWindow="500" windowWidth="34040" windowHeight="20320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="4980" windowWidth="33600" windowHeight="19080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metro_budget" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="93">
   <si>
     <t>Department</t>
   </si>
@@ -260,15 +260,6 @@
     <t>Trustee</t>
   </si>
   <si>
-    <t>Question 3</t>
-  </si>
-  <si>
-    <t>Question 4</t>
-  </si>
-  <si>
-    <t>Question 5</t>
-  </si>
-  <si>
     <t>Question 6</t>
   </si>
   <si>
@@ -329,7 +320,22 @@
     <t>Actual spending amount - budget amount for fiscal year 2019</t>
   </si>
   <si>
-    <t>Question 7</t>
+    <t>Question 3 (VLOOKUP)</t>
+  </si>
+  <si>
+    <t>Question 4 (XLOOKUP)</t>
+  </si>
+  <si>
+    <t>Question 5 (INDEX/MATCH)</t>
+  </si>
+  <si>
+    <t>Two Way Lookup</t>
+  </si>
+  <si>
+    <t>Question 7 (VLOOKUP/MATCH)</t>
+  </si>
+  <si>
+    <t>(Double XLOOKUP)</t>
   </si>
 </sst>
 </file>
@@ -480,11 +486,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -860,7 +868,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -875,8 +883,6 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -1233,10 +1239,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P100"/>
+  <dimension ref="A1:P107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="G74" sqref="G74"/>
+    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
+      <selection activeCell="G100" sqref="G100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1244,7 +1250,7 @@
     <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="26.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.83203125" customWidth="1"/>
-    <col min="6" max="6" width="28.6640625" customWidth="1"/>
+    <col min="6" max="6" width="23.5" customWidth="1"/>
     <col min="7" max="7" width="15.5" customWidth="1"/>
     <col min="8" max="8" width="26.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="12" width="15.83203125" customWidth="1"/>
@@ -1254,7 +1260,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
@@ -1287,19 +1293,19 @@
       <c r="K1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="M1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="N1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="O1" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="P1" s="12" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1307,23 +1313,23 @@
       <c r="A2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2">
         <v>356640100</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2">
         <v>341243679.13</v>
       </c>
-      <c r="D2" s="12">
-        <f>C2-B2</f>
+      <c r="D2">
+        <f t="shared" ref="D2:D52" si="0">C2-B2</f>
         <v>-15396420.870000005</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="5">
         <f>IFERROR(D2/B2,0)</f>
         <v>-4.3170750765267295E-2</v>
       </c>
-      <c r="F2" s="12">
-        <f>RANK(E2,E:E,0)</f>
-        <v>38</v>
+      <c r="F2">
+        <f>IF(E2=0,"",RANK(E2,$E$2:$E$52,1))</f>
+        <v>14</v>
       </c>
       <c r="G2">
         <v>382685200</v>
@@ -1340,8 +1346,8 @@
         <v>-9.4972027086493035E-2</v>
       </c>
       <c r="K2">
-        <f>RANK(J2,J:J,0)</f>
-        <v>42</v>
+        <f>IF(J2=0,"",RANK(J2,$J$2:$J$52,1))</f>
+        <v>10</v>
       </c>
       <c r="L2">
         <v>376548600</v>
@@ -1358,31 +1364,31 @@
         <v>-5.6484362894991494E-2</v>
       </c>
       <c r="P2">
-        <f>RANK(O2,O:O,0)</f>
-        <v>38</v>
+        <f>IF(O2=0,"",RANK(O2,$O$2:$O$52,1))</f>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3">
         <v>328800</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3">
         <v>321214.59000000003</v>
       </c>
-      <c r="D3" s="12">
-        <f t="shared" ref="D3:D52" si="0">C3-B3</f>
+      <c r="D3">
+        <f t="shared" si="0"/>
         <v>-7585.4099999999744</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="5">
         <f t="shared" ref="E3:E52" si="1">IFERROR(D3/B3,0)</f>
         <v>-2.3069981751824741E-2</v>
       </c>
-      <c r="F3" s="12">
-        <f t="shared" ref="F3:F52" si="2">RANK(E3,E:E,0)</f>
-        <v>30</v>
+      <c r="F3">
+        <f t="shared" ref="F3:F52" si="2">IF(E3=0,"",RANK(E3,$E$2:$E$52,1))</f>
+        <v>22</v>
       </c>
       <c r="G3">
         <v>334800</v>
@@ -1399,8 +1405,8 @@
         <v>-6.6804928315415249E-2</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K52" si="5">RANK(J3,J:J,0)</f>
-        <v>38</v>
+        <f t="shared" ref="K3:K52" si="5">IF(J3=0,"",RANK(J3,$J$2:$J$52,1))</f>
+        <v>14</v>
       </c>
       <c r="L3">
         <v>322700</v>
@@ -1417,31 +1423,31 @@
         <v>-1.3540749922529313E-3</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3:P52" si="8">RANK(O3,O:O,0)</f>
-        <v>15</v>
+        <f t="shared" ref="P3:P52" si="8">IF(O3=0,"",RANK(O3,$O$2:$O$52,1))</f>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4">
         <v>3130600</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4">
         <v>3115157.5599999898</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4">
         <f t="shared" si="0"/>
         <v>-15442.440000010189</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="5">
         <f t="shared" si="1"/>
         <v>-4.9327413275443007E-3</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="G4">
         <v>3652300</v>
@@ -1459,7 +1465,7 @@
       </c>
       <c r="K4">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="L4">
         <v>3662400</v>
@@ -1477,30 +1483,30 @@
       </c>
       <c r="P4">
         <f t="shared" si="8"/>
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5">
         <v>7670700</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5">
         <v>6947552.6699999999</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5">
         <f t="shared" si="0"/>
         <v>-723147.33000000007</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="5">
         <f t="shared" si="1"/>
         <v>-9.4273968477453174E-2</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5">
         <f t="shared" si="2"/>
-        <v>48</v>
+        <v>4</v>
       </c>
       <c r="G5">
         <v>7968300</v>
@@ -1518,7 +1524,7 @@
       </c>
       <c r="K5">
         <f t="shared" si="5"/>
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="L5">
         <v>7759600</v>
@@ -1536,30 +1542,30 @@
       </c>
       <c r="P5">
         <f t="shared" si="8"/>
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6">
         <v>409300</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6">
         <v>385908.52</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6">
         <f t="shared" si="0"/>
         <v>-23391.479999999981</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="5">
         <f t="shared" si="1"/>
         <v>-5.7149963352064452E-2</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6">
         <f t="shared" si="2"/>
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="G6">
         <v>428500</v>
@@ -1577,7 +1583,7 @@
       </c>
       <c r="K6">
         <f t="shared" si="5"/>
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="L6">
         <v>445200</v>
@@ -1595,30 +1601,30 @@
       </c>
       <c r="P6">
         <f t="shared" si="8"/>
-        <v>13</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7">
         <v>3329000</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7">
         <v>2946071.21</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7">
         <f t="shared" si="0"/>
         <v>-382928.79000000004</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="5">
         <f t="shared" si="1"/>
         <v>-0.11502817362571344</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7">
         <f t="shared" si="2"/>
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="G7">
         <v>3390900</v>
@@ -1636,7 +1642,7 @@
       </c>
       <c r="K7">
         <f t="shared" si="5"/>
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="L7">
         <v>3345200</v>
@@ -1654,30 +1660,30 @@
       </c>
       <c r="P7">
         <f t="shared" si="8"/>
-        <v>48</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8">
         <v>1552100</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8">
         <v>1315623.30999999</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8">
         <f t="shared" si="0"/>
         <v>-236476.69000000996</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="5">
         <f t="shared" si="1"/>
         <v>-0.15235918433091292</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>1</v>
       </c>
       <c r="G8">
         <v>1590700</v>
@@ -1695,7 +1701,7 @@
       </c>
       <c r="K8">
         <f t="shared" si="5"/>
-        <v>48</v>
+        <v>4</v>
       </c>
       <c r="L8">
         <v>1579300</v>
@@ -1713,30 +1719,30 @@
       </c>
       <c r="P8">
         <f t="shared" si="8"/>
-        <v>50</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9">
         <v>9349400</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9">
         <v>8952825.2799999993</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9">
         <f t="shared" si="0"/>
         <v>-396574.72000000067</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="5">
         <f t="shared" si="1"/>
         <v>-4.2417130511048909E-2</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9">
         <f t="shared" si="2"/>
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="G9">
         <v>11073700</v>
@@ -1754,7 +1760,7 @@
       </c>
       <c r="K9">
         <f t="shared" si="5"/>
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="L9">
         <v>10790500</v>
@@ -1772,30 +1778,30 @@
       </c>
       <c r="P9">
         <f t="shared" si="8"/>
-        <v>43</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10">
         <v>443300</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10">
         <v>407090.37</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10">
         <f t="shared" si="0"/>
         <v>-36209.630000000005</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="5">
         <f t="shared" si="1"/>
         <v>-8.1681998646514792E-2</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10">
         <f t="shared" si="2"/>
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="G10">
         <v>495200</v>
@@ -1813,7 +1819,7 @@
       </c>
       <c r="K10">
         <f t="shared" si="5"/>
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="L10">
         <v>487500</v>
@@ -1831,30 +1837,30 @@
       </c>
       <c r="P10">
         <f t="shared" si="8"/>
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="12">
-        <v>0</v>
-      </c>
-      <c r="C11" s="12">
-        <v>0</v>
-      </c>
-      <c r="D11" s="12">
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" t="str">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v/>
       </c>
       <c r="G11">
         <v>0</v>
@@ -1870,9 +1876,9 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K11">
+      <c r="K11" t="str">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="L11">
         <v>375000</v>
@@ -1890,30 +1896,30 @@
       </c>
       <c r="P11">
         <f t="shared" si="8"/>
-        <v>51</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12">
         <v>4280900</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12">
         <v>4066595.33</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12">
         <f t="shared" si="0"/>
         <v>-214304.66999999993</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="5">
         <f t="shared" si="1"/>
         <v>-5.0060657805601608E-2</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12">
         <f t="shared" si="2"/>
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="G12">
         <v>4700400</v>
@@ -1931,7 +1937,7 @@
       </c>
       <c r="K12">
         <f t="shared" si="5"/>
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="L12">
         <v>4677800</v>
@@ -1949,30 +1955,30 @@
       </c>
       <c r="P12">
         <f t="shared" si="8"/>
-        <v>42</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13">
         <v>5847800</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13">
         <v>5772288.3300000001</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D13">
         <f t="shared" si="0"/>
         <v>-75511.669999999925</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="5">
         <f t="shared" si="1"/>
         <v>-1.2912833886247806E-2</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F13">
         <f t="shared" si="2"/>
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="G13">
         <v>6223700</v>
@@ -1990,7 +1996,7 @@
       </c>
       <c r="K13">
         <f t="shared" si="5"/>
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="L13">
         <v>6207300</v>
@@ -2008,30 +2014,30 @@
       </c>
       <c r="P13">
         <f t="shared" si="8"/>
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14">
         <v>512000</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14">
         <v>505017.37</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14">
         <f t="shared" si="0"/>
         <v>-6982.6300000000047</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="5">
         <f t="shared" si="1"/>
         <v>-1.3637949218750009E-2</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="G14">
         <v>530500</v>
@@ -2049,7 +2055,7 @@
       </c>
       <c r="K14">
         <f t="shared" si="5"/>
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="L14">
         <v>526200</v>
@@ -2067,30 +2073,30 @@
       </c>
       <c r="P14">
         <f t="shared" si="8"/>
-        <v>33</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15">
         <v>156049100</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15">
         <v>156545919.90000001</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15">
         <f t="shared" si="0"/>
         <v>496819.90000000596</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="5">
         <f t="shared" si="1"/>
         <v>3.1837408866824991E-3</v>
       </c>
-      <c r="F15" s="12">
+      <c r="F15">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="G15">
         <v>184167800</v>
@@ -2108,7 +2114,7 @@
       </c>
       <c r="K15">
         <f t="shared" si="5"/>
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="L15">
         <v>188953500</v>
@@ -2126,30 +2132,30 @@
       </c>
       <c r="P15">
         <f t="shared" si="8"/>
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B16">
         <v>6600700</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C16">
         <v>6522480.4599999897</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16">
         <f t="shared" si="0"/>
         <v>-78219.540000010282</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="5">
         <f t="shared" si="1"/>
         <v>-1.1850188616360429E-2</v>
       </c>
-      <c r="F16" s="12">
+      <c r="F16">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="G16">
         <v>7352500</v>
@@ -2167,7 +2173,7 @@
       </c>
       <c r="K16">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="L16">
         <v>7397200</v>
@@ -2185,30 +2191,30 @@
       </c>
       <c r="P16">
         <f t="shared" si="8"/>
-        <v>9</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17">
         <v>14860800</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17">
         <v>14439480.050000001</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17">
         <f t="shared" si="0"/>
         <v>-421319.94999999925</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="5">
         <f t="shared" si="1"/>
         <v>-2.8351094826658003E-2</v>
       </c>
-      <c r="F17" s="12">
+      <c r="F17">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="G17">
         <v>15309700</v>
@@ -2226,7 +2232,7 @@
       </c>
       <c r="K17">
         <f t="shared" si="5"/>
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L17">
         <v>15311800</v>
@@ -2244,30 +2250,30 @@
       </c>
       <c r="P17">
         <f t="shared" si="8"/>
-        <v>41</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="12">
+      <c r="B18">
         <v>2764700</v>
       </c>
-      <c r="C18" s="12">
+      <c r="C18">
         <v>2615303.8999999901</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D18">
         <f t="shared" si="0"/>
         <v>-149396.10000000987</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="5">
         <f t="shared" si="1"/>
         <v>-5.4037002206391245E-2</v>
       </c>
-      <c r="F18" s="12">
+      <c r="F18">
         <f t="shared" si="2"/>
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="G18">
         <v>2861000</v>
@@ -2285,7 +2291,7 @@
       </c>
       <c r="K18">
         <f t="shared" si="5"/>
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="L18">
         <v>2910600</v>
@@ -2303,30 +2309,30 @@
       </c>
       <c r="P18">
         <f t="shared" si="8"/>
-        <v>49</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="12">
+      <c r="B19">
         <v>8837300</v>
       </c>
-      <c r="C19" s="12">
+      <c r="C19">
         <v>8460963.1999999899</v>
       </c>
-      <c r="D19" s="12">
+      <c r="D19">
         <f t="shared" si="0"/>
         <v>-376336.80000001006</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E19" s="5">
         <f t="shared" si="1"/>
         <v>-4.258504294298146E-2</v>
       </c>
-      <c r="F19" s="12">
+      <c r="F19">
         <f t="shared" si="2"/>
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="G19">
         <v>9713300</v>
@@ -2344,7 +2350,7 @@
       </c>
       <c r="K19">
         <f t="shared" si="5"/>
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="L19">
         <v>9343000</v>
@@ -2362,30 +2368,30 @@
       </c>
       <c r="P19">
         <f t="shared" si="8"/>
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="12">
+      <c r="B20">
         <v>124385900</v>
       </c>
-      <c r="C20" s="12">
+      <c r="C20">
         <v>124384360.159999</v>
       </c>
-      <c r="D20" s="12">
+      <c r="D20">
         <f t="shared" si="0"/>
         <v>-1539.8400010019541</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E20" s="5">
         <f t="shared" si="1"/>
         <v>-1.2379538203300809E-5</v>
       </c>
-      <c r="F20" s="12">
+      <c r="F20">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="G20">
         <v>131849400</v>
@@ -2403,7 +2409,7 @@
       </c>
       <c r="K20">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="L20">
         <v>130621400</v>
@@ -2421,30 +2427,30 @@
       </c>
       <c r="P20">
         <f t="shared" si="8"/>
-        <v>6</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="12">
+      <c r="B21">
         <v>24332100</v>
       </c>
-      <c r="C21" s="12">
+      <c r="C21">
         <v>22408587.5499999</v>
       </c>
-      <c r="D21" s="12">
+      <c r="D21">
         <f t="shared" si="0"/>
         <v>-1923512.4500000998</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E21" s="5">
         <f t="shared" si="1"/>
         <v>-7.9052463618023094E-2</v>
       </c>
-      <c r="F21" s="12">
+      <c r="F21">
         <f t="shared" si="2"/>
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="G21">
         <v>24497400</v>
@@ -2462,7 +2468,7 @@
       </c>
       <c r="K21">
         <f t="shared" si="5"/>
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="L21">
         <v>24323000</v>
@@ -2480,30 +2486,30 @@
       </c>
       <c r="P21">
         <f t="shared" si="8"/>
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="12">
+      <c r="B22">
         <v>11566000</v>
       </c>
-      <c r="C22" s="12">
+      <c r="C22">
         <v>11412339.8799999</v>
       </c>
-      <c r="D22" s="12">
+      <c r="D22">
         <f t="shared" si="0"/>
         <v>-153660.12000009976</v>
       </c>
-      <c r="E22" s="13">
+      <c r="E22" s="5">
         <f t="shared" si="1"/>
         <v>-1.3285502334437123E-2</v>
       </c>
-      <c r="F22" s="12">
+      <c r="F22">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="G22">
         <v>11980700</v>
@@ -2521,7 +2527,7 @@
       </c>
       <c r="K22">
         <f t="shared" si="5"/>
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="L22">
         <v>11935200</v>
@@ -2539,30 +2545,30 @@
       </c>
       <c r="P22">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="12">
+      <c r="B23">
         <v>20862700</v>
       </c>
-      <c r="C23" s="12">
+      <c r="C23">
         <v>20036743.4099999</v>
       </c>
-      <c r="D23" s="12">
+      <c r="D23">
         <f t="shared" si="0"/>
         <v>-825956.59000010043</v>
       </c>
-      <c r="E23" s="13">
+      <c r="E23" s="5">
         <f t="shared" si="1"/>
         <v>-3.9590110100806722E-2</v>
       </c>
-      <c r="F23" s="12">
+      <c r="F23">
         <f t="shared" si="2"/>
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="G23">
         <v>22683800</v>
@@ -2605,23 +2611,23 @@
       <c r="A24" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="12">
+      <c r="B24">
         <v>917200</v>
       </c>
-      <c r="C24" s="12">
+      <c r="C24">
         <v>904969.19</v>
       </c>
-      <c r="D24" s="12">
+      <c r="D24">
         <f t="shared" si="0"/>
         <v>-12230.810000000056</v>
       </c>
-      <c r="E24" s="13">
+      <c r="E24" s="5">
         <f t="shared" si="1"/>
         <v>-1.3334943305713101E-2</v>
       </c>
-      <c r="F24" s="12">
+      <c r="F24">
         <f t="shared" si="2"/>
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="G24">
         <v>1112700</v>
@@ -2639,7 +2645,7 @@
       </c>
       <c r="K24">
         <f t="shared" si="5"/>
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="L24">
         <v>1112600</v>
@@ -2657,30 +2663,30 @@
       </c>
       <c r="P24">
         <f t="shared" si="8"/>
-        <v>11</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="12">
+      <c r="B25">
         <v>484100</v>
       </c>
-      <c r="C25" s="12">
+      <c r="C25">
         <v>479149.53</v>
       </c>
-      <c r="D25" s="12">
+      <c r="D25">
         <f t="shared" si="0"/>
         <v>-4950.4699999999721</v>
       </c>
-      <c r="E25" s="13">
+      <c r="E25" s="5">
         <f t="shared" si="1"/>
         <v>-1.0226130964676661E-2</v>
       </c>
-      <c r="F25" s="12">
+      <c r="F25">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="G25">
         <v>505200</v>
@@ -2698,7 +2704,7 @@
       </c>
       <c r="K25">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="L25">
         <v>496500</v>
@@ -2716,30 +2722,30 @@
       </c>
       <c r="P25">
         <f t="shared" si="8"/>
-        <v>17</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="12">
+      <c r="B26">
         <v>5249800</v>
       </c>
-      <c r="C26" s="12">
+      <c r="C26">
         <v>4801960.08</v>
       </c>
-      <c r="D26" s="12">
+      <c r="D26">
         <f t="shared" si="0"/>
         <v>-447839.91999999993</v>
       </c>
-      <c r="E26" s="13">
+      <c r="E26" s="5">
         <f t="shared" si="1"/>
         <v>-8.5306091660634673E-2</v>
       </c>
-      <c r="F26" s="12">
+      <c r="F26">
         <f t="shared" si="2"/>
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="G26">
         <v>5442200</v>
@@ -2757,7 +2763,7 @@
       </c>
       <c r="K26">
         <f t="shared" si="5"/>
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="L26">
         <v>5430700</v>
@@ -2775,30 +2781,30 @@
       </c>
       <c r="P26">
         <f t="shared" si="8"/>
-        <v>39</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>41</v>
       </c>
-      <c r="B27" s="12">
-        <v>0</v>
-      </c>
-      <c r="C27" s="12">
-        <v>0</v>
-      </c>
-      <c r="D27" s="12">
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E27" s="13">
+      <c r="E27" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F27" s="12">
+      <c r="F27" t="str">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v/>
       </c>
       <c r="G27">
         <v>0</v>
@@ -2814,9 +2820,9 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K27">
+      <c r="K27" t="str">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="L27">
         <v>0</v>
@@ -2832,32 +2838,32 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="P27">
+      <c r="P27" t="str">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="12">
+      <c r="B28">
         <v>1382900</v>
       </c>
-      <c r="C28" s="12">
+      <c r="C28">
         <v>1250442.02</v>
       </c>
-      <c r="D28" s="12">
+      <c r="D28">
         <f t="shared" si="0"/>
         <v>-132457.97999999998</v>
       </c>
-      <c r="E28" s="13">
+      <c r="E28" s="5">
         <f t="shared" si="1"/>
         <v>-9.5782760864849215E-2</v>
       </c>
-      <c r="F28" s="12">
+      <c r="F28">
         <f t="shared" si="2"/>
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="G28">
         <v>1545700</v>
@@ -2875,7 +2881,7 @@
       </c>
       <c r="K28">
         <f t="shared" si="5"/>
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="L28">
         <v>1525900</v>
@@ -2893,30 +2899,30 @@
       </c>
       <c r="P28">
         <f t="shared" si="8"/>
-        <v>45</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="12">
+      <c r="B29">
         <v>2561800</v>
       </c>
-      <c r="C29" s="12">
+      <c r="C29">
         <v>2523884.71</v>
       </c>
-      <c r="D29" s="12">
+      <c r="D29">
         <f t="shared" si="0"/>
         <v>-37915.290000000037</v>
       </c>
-      <c r="E29" s="13">
+      <c r="E29" s="5">
         <f t="shared" si="1"/>
         <v>-1.4800253727847622E-2</v>
       </c>
-      <c r="F29" s="12">
+      <c r="F29">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G29">
         <v>2779500</v>
@@ -2934,7 +2940,7 @@
       </c>
       <c r="K29">
         <f t="shared" si="5"/>
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="L29">
         <v>2889900</v>
@@ -2952,30 +2958,30 @@
       </c>
       <c r="P29">
         <f t="shared" si="8"/>
-        <v>8</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>44</v>
       </c>
-      <c r="B30" s="12">
+      <c r="B30">
         <v>12132200</v>
       </c>
-      <c r="C30" s="12">
+      <c r="C30">
         <v>12030494.1</v>
       </c>
-      <c r="D30" s="12">
+      <c r="D30">
         <f t="shared" si="0"/>
         <v>-101705.90000000037</v>
       </c>
-      <c r="E30" s="13">
+      <c r="E30" s="5">
         <f t="shared" si="1"/>
         <v>-8.3831374359143746E-3</v>
       </c>
-      <c r="F30" s="12">
+      <c r="F30">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="G30">
         <v>12735900</v>
@@ -2993,7 +2999,7 @@
       </c>
       <c r="K30">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="L30">
         <v>12861300</v>
@@ -3011,30 +3017,30 @@
       </c>
       <c r="P30">
         <f t="shared" si="8"/>
-        <v>16</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>45</v>
       </c>
-      <c r="B31" s="12">
+      <c r="B31">
         <v>1765600</v>
       </c>
-      <c r="C31" s="12">
+      <c r="C31">
         <v>1740827.69</v>
       </c>
-      <c r="D31" s="12">
+      <c r="D31">
         <f t="shared" si="0"/>
         <v>-24772.310000000056</v>
       </c>
-      <c r="E31" s="13">
+      <c r="E31" s="5">
         <f t="shared" si="1"/>
         <v>-1.4030533529678329E-2</v>
       </c>
-      <c r="F31" s="12">
+      <c r="F31">
         <f t="shared" si="2"/>
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G31">
         <v>1823300</v>
@@ -3052,7 +3058,7 @@
       </c>
       <c r="K31">
         <f t="shared" si="5"/>
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="L31">
         <v>1870700</v>
@@ -3070,30 +3076,30 @@
       </c>
       <c r="P31">
         <f t="shared" si="8"/>
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>46</v>
       </c>
-      <c r="B32" s="12">
+      <c r="B32">
         <v>5999400</v>
       </c>
-      <c r="C32" s="12">
+      <c r="C32">
         <v>5925637.7199999904</v>
       </c>
-      <c r="D32" s="12">
+      <c r="D32">
         <f t="shared" si="0"/>
         <v>-73762.280000009574</v>
       </c>
-      <c r="E32" s="13">
+      <c r="E32" s="5">
         <f t="shared" si="1"/>
         <v>-1.2294942827617691E-2</v>
       </c>
-      <c r="F32" s="12">
+      <c r="F32">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="G32">
         <v>6195500</v>
@@ -3111,7 +3117,7 @@
       </c>
       <c r="K32">
         <f t="shared" si="5"/>
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="L32">
         <v>6157400</v>
@@ -3129,30 +3135,30 @@
       </c>
       <c r="P32">
         <f t="shared" si="8"/>
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>47</v>
       </c>
-      <c r="B33" s="12">
+      <c r="B33">
         <v>927703099.99999905</v>
       </c>
-      <c r="C33" s="12">
+      <c r="C33">
         <v>920284264.73000002</v>
       </c>
-      <c r="D33" s="12">
+      <c r="D33">
         <f t="shared" si="0"/>
         <v>-7418835.2699990273</v>
       </c>
-      <c r="E33" s="13">
+      <c r="E33" s="5">
         <f t="shared" si="1"/>
         <v>-7.9969930789269058E-3</v>
       </c>
-      <c r="F33" s="12">
+      <c r="F33">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="G33">
         <v>979671000</v>
@@ -3170,7 +3176,7 @@
       </c>
       <c r="K33">
         <f t="shared" si="5"/>
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="L33">
         <v>989572899.99999905</v>
@@ -3188,28 +3194,28 @@
       </c>
       <c r="P33">
         <f t="shared" si="8"/>
-        <v>18</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>48</v>
       </c>
-      <c r="B34" s="12">
+      <c r="B34">
         <v>4189300</v>
       </c>
-      <c r="C34" s="12">
+      <c r="C34">
         <v>4109958.22</v>
       </c>
-      <c r="D34" s="12">
+      <c r="D34">
         <f t="shared" si="0"/>
         <v>-79341.779999999795</v>
       </c>
-      <c r="E34" s="13">
+      <c r="E34" s="5">
         <f t="shared" si="1"/>
         <v>-1.8939149738619768E-2</v>
       </c>
-      <c r="F34" s="12">
+      <c r="F34">
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
@@ -3229,7 +3235,7 @@
       </c>
       <c r="K34">
         <f t="shared" si="5"/>
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="L34">
         <v>4345600</v>
@@ -3247,30 +3253,30 @@
       </c>
       <c r="P34">
         <f t="shared" si="8"/>
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>49</v>
       </c>
-      <c r="B35" s="12">
-        <v>0</v>
-      </c>
-      <c r="C35" s="12">
-        <v>0</v>
-      </c>
-      <c r="D35" s="12">
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E35" s="13">
+      <c r="E35" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F35" s="12">
+      <c r="F35" t="str">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v/>
       </c>
       <c r="G35">
         <v>0</v>
@@ -3286,9 +3292,9 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K35">
+      <c r="K35" t="str">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="L35">
         <v>0</v>
@@ -3304,32 +3310,32 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="P35">
+      <c r="P35" t="str">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>50</v>
       </c>
-      <c r="B36" s="12">
+      <c r="B36">
         <v>798200</v>
       </c>
-      <c r="C36" s="12">
+      <c r="C36">
         <v>735423.27999999898</v>
       </c>
-      <c r="D36" s="12">
+      <c r="D36">
         <f t="shared" si="0"/>
         <v>-62776.72000000102</v>
       </c>
-      <c r="E36" s="13">
+      <c r="E36" s="5">
         <f t="shared" si="1"/>
         <v>-7.8647857679780775E-2</v>
       </c>
-      <c r="F36" s="12">
+      <c r="F36">
         <f t="shared" si="2"/>
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="G36">
         <v>898700</v>
@@ -3347,7 +3353,7 @@
       </c>
       <c r="K36">
         <f t="shared" si="5"/>
-        <v>51</v>
+        <v>1</v>
       </c>
       <c r="L36">
         <v>878300</v>
@@ -3365,30 +3371,30 @@
       </c>
       <c r="P36">
         <f t="shared" si="8"/>
-        <v>47</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>51</v>
       </c>
-      <c r="B37" s="12">
+      <c r="B37">
         <v>2087800</v>
       </c>
-      <c r="C37" s="12">
+      <c r="C37">
         <v>2005447.73999999</v>
       </c>
-      <c r="D37" s="12">
+      <c r="D37">
         <f t="shared" si="0"/>
         <v>-82352.260000010021</v>
       </c>
-      <c r="E37" s="13">
+      <c r="E37" s="5">
         <f t="shared" si="1"/>
         <v>-3.9444515758219188E-2</v>
       </c>
-      <c r="F37" s="12">
+      <c r="F37">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="G37">
         <v>2229200</v>
@@ -3406,7 +3412,7 @@
       </c>
       <c r="K37">
         <f t="shared" si="5"/>
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="L37">
         <v>2296900</v>
@@ -3424,30 +3430,30 @@
       </c>
       <c r="P37">
         <f t="shared" si="8"/>
-        <v>44</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>52</v>
       </c>
-      <c r="B38" s="12">
+      <c r="B38">
         <v>855300</v>
       </c>
-      <c r="C38" s="12">
+      <c r="C38">
         <v>838669.82</v>
       </c>
-      <c r="D38" s="12">
+      <c r="D38">
         <f t="shared" si="0"/>
         <v>-16630.180000000051</v>
       </c>
-      <c r="E38" s="13">
+      <c r="E38" s="5">
         <f t="shared" si="1"/>
         <v>-1.9443680579913542E-2</v>
       </c>
-      <c r="F38" s="12">
+      <c r="F38">
         <f t="shared" si="2"/>
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G38">
         <v>792800</v>
@@ -3465,7 +3471,7 @@
       </c>
       <c r="K38">
         <f t="shared" si="5"/>
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="L38">
         <v>777800</v>
@@ -3483,30 +3489,30 @@
       </c>
       <c r="P38">
         <f t="shared" si="8"/>
-        <v>12</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>53</v>
       </c>
-      <c r="B39" s="12">
+      <c r="B39">
         <v>883900</v>
       </c>
-      <c r="C39" s="12">
+      <c r="C39">
         <v>813108.87</v>
       </c>
-      <c r="D39" s="12">
+      <c r="D39">
         <f t="shared" si="0"/>
         <v>-70791.13</v>
       </c>
-      <c r="E39" s="13">
+      <c r="E39" s="5">
         <f t="shared" si="1"/>
         <v>-8.008952370177623E-2</v>
       </c>
-      <c r="F39" s="12">
+      <c r="F39">
         <f t="shared" si="2"/>
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="G39">
         <v>1294400</v>
@@ -3524,7 +3530,7 @@
       </c>
       <c r="K39">
         <f t="shared" si="5"/>
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="L39">
         <v>1759500</v>
@@ -3542,30 +3548,30 @@
       </c>
       <c r="P39">
         <f t="shared" si="8"/>
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>54</v>
       </c>
-      <c r="B40" s="12">
+      <c r="B40">
         <v>38381900</v>
       </c>
-      <c r="C40" s="12">
+      <c r="C40">
         <v>37565141.859999903</v>
       </c>
-      <c r="D40" s="12">
+      <c r="D40">
         <f t="shared" si="0"/>
         <v>-816758.14000009745</v>
       </c>
-      <c r="E40" s="13">
+      <c r="E40" s="5">
         <f t="shared" si="1"/>
         <v>-2.1279773539092578E-2</v>
       </c>
-      <c r="F40" s="12">
+      <c r="F40">
         <f t="shared" si="2"/>
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="G40">
         <v>39964900</v>
@@ -3583,7 +3589,7 @@
       </c>
       <c r="K40">
         <f t="shared" si="5"/>
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="L40">
         <v>40216700</v>
@@ -3601,30 +3607,30 @@
       </c>
       <c r="P40">
         <f t="shared" si="8"/>
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>55</v>
       </c>
-      <c r="B41" s="12">
+      <c r="B41">
         <v>4593300</v>
       </c>
-      <c r="C41" s="12">
+      <c r="C41">
         <v>4409060.2099999897</v>
       </c>
-      <c r="D41" s="12">
+      <c r="D41">
         <f t="shared" si="0"/>
         <v>-184239.79000001028</v>
       </c>
-      <c r="E41" s="13">
+      <c r="E41" s="5">
         <f t="shared" si="1"/>
         <v>-4.0110550149132493E-2</v>
       </c>
-      <c r="F41" s="12">
+      <c r="F41">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="G41">
         <v>5089500</v>
@@ -3642,7 +3648,7 @@
       </c>
       <c r="K41">
         <f t="shared" si="5"/>
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="L41">
         <v>4799900</v>
@@ -3660,30 +3666,30 @@
       </c>
       <c r="P41">
         <f t="shared" si="8"/>
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>56</v>
       </c>
-      <c r="B42" s="12">
+      <c r="B42">
         <v>188593300</v>
       </c>
-      <c r="C42" s="12">
+      <c r="C42">
         <v>188551675.67999899</v>
       </c>
-      <c r="D42" s="12">
+      <c r="D42">
         <f t="shared" si="0"/>
         <v>-41624.320001006126</v>
       </c>
-      <c r="E42" s="13">
+      <c r="E42" s="5">
         <f t="shared" si="1"/>
         <v>-2.2070943135841053E-4</v>
       </c>
-      <c r="F42" s="12">
+      <c r="F42">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="G42">
         <v>199130300</v>
@@ -3701,7 +3707,7 @@
       </c>
       <c r="K42">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="L42">
         <v>199954600</v>
@@ -3719,30 +3725,30 @@
       </c>
       <c r="P42">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>57</v>
       </c>
-      <c r="B43" s="12">
+      <c r="B43">
         <v>8135400</v>
       </c>
-      <c r="C43" s="12">
+      <c r="C43">
         <v>7968645.8300000001</v>
       </c>
-      <c r="D43" s="12">
+      <c r="D43">
         <f t="shared" si="0"/>
         <v>-166754.16999999993</v>
       </c>
-      <c r="E43" s="13">
+      <c r="E43" s="5">
         <f t="shared" si="1"/>
         <v>-2.0497353541313264E-2</v>
       </c>
-      <c r="F43" s="12">
+      <c r="F43">
         <f t="shared" si="2"/>
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="G43">
         <v>8560800</v>
@@ -3760,7 +3766,7 @@
       </c>
       <c r="K43">
         <f t="shared" si="5"/>
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="L43">
         <v>8497500</v>
@@ -3778,30 +3784,30 @@
       </c>
       <c r="P43">
         <f t="shared" si="8"/>
-        <v>34</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>58</v>
       </c>
-      <c r="B44" s="12">
+      <c r="B44">
         <v>30083200</v>
       </c>
-      <c r="C44" s="12">
+      <c r="C44">
         <v>29789104.379999999</v>
       </c>
-      <c r="D44" s="12">
+      <c r="D44">
         <f t="shared" si="0"/>
         <v>-294095.62000000104</v>
       </c>
-      <c r="E44" s="13">
+      <c r="E44" s="5">
         <f t="shared" si="1"/>
         <v>-9.7760750186150751E-3</v>
       </c>
-      <c r="F44" s="12">
+      <c r="F44">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="G44">
         <v>31040700</v>
@@ -3819,7 +3825,7 @@
       </c>
       <c r="K44">
         <f t="shared" si="5"/>
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="L44">
         <v>31282200</v>
@@ -3837,30 +3843,30 @@
       </c>
       <c r="P44">
         <f t="shared" si="8"/>
-        <v>7</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>59</v>
       </c>
-      <c r="B45" s="12">
+      <c r="B45">
         <v>55301600</v>
       </c>
-      <c r="C45" s="12">
+      <c r="C45">
         <v>54589584.0499999</v>
       </c>
-      <c r="D45" s="12">
+      <c r="D45">
         <f t="shared" si="0"/>
         <v>-712015.95000009984</v>
       </c>
-      <c r="E45" s="13">
+      <c r="E45" s="5">
         <f t="shared" si="1"/>
         <v>-1.287514194887851E-2</v>
       </c>
-      <c r="F45" s="12">
+      <c r="F45">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="G45">
         <v>56792200</v>
@@ -3878,7 +3884,7 @@
       </c>
       <c r="K45">
         <f t="shared" si="5"/>
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="L45">
         <v>56027100</v>
@@ -3896,30 +3902,30 @@
       </c>
       <c r="P45">
         <f t="shared" si="8"/>
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>60</v>
       </c>
-      <c r="B46" s="12">
+      <c r="B46">
         <v>259100</v>
       </c>
-      <c r="C46" s="12">
+      <c r="C46">
         <v>258322.43</v>
       </c>
-      <c r="D46" s="12">
+      <c r="D46">
         <f t="shared" si="0"/>
         <v>-777.57000000000698</v>
       </c>
-      <c r="E46" s="13">
+      <c r="E46" s="5">
         <f t="shared" si="1"/>
         <v>-3.0010420686993711E-3</v>
       </c>
-      <c r="F46" s="12">
+      <c r="F46">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="G46">
         <v>266000</v>
@@ -3937,7 +3943,7 @@
       </c>
       <c r="K46">
         <f t="shared" si="5"/>
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="L46">
         <v>267100</v>
@@ -3955,30 +3961,30 @@
       </c>
       <c r="P46">
         <f t="shared" si="8"/>
-        <v>36</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>61</v>
       </c>
-      <c r="B47" s="12">
+      <c r="B47">
         <v>70390700</v>
       </c>
-      <c r="C47" s="12">
+      <c r="C47">
         <v>70378426.719999999</v>
       </c>
-      <c r="D47" s="12">
+      <c r="D47">
         <f t="shared" si="0"/>
         <v>-12273.280000001192</v>
       </c>
-      <c r="E47" s="13">
+      <c r="E47" s="5">
         <f t="shared" si="1"/>
         <v>-1.7435939690898361E-4</v>
       </c>
-      <c r="F47" s="12">
+      <c r="F47">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="G47">
         <v>73467000</v>
@@ -3996,7 +4002,7 @@
       </c>
       <c r="K47">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="L47">
         <v>75072800</v>
@@ -4014,30 +4020,30 @@
       </c>
       <c r="P47">
         <f t="shared" si="8"/>
-        <v>14</v>
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>62</v>
       </c>
-      <c r="B48" s="12">
+      <c r="B48">
         <v>6737100</v>
       </c>
-      <c r="C48" s="12">
+      <c r="C48">
         <v>6527352.5699999901</v>
       </c>
-      <c r="D48" s="12">
+      <c r="D48">
         <f t="shared" si="0"/>
         <v>-209747.43000000995</v>
       </c>
-      <c r="E48" s="13">
+      <c r="E48" s="5">
         <f t="shared" si="1"/>
         <v>-3.1133192323107857E-2</v>
       </c>
-      <c r="F48" s="12">
+      <c r="F48">
         <f t="shared" si="2"/>
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="G48">
         <v>7214700</v>
@@ -4055,7 +4061,7 @@
       </c>
       <c r="K48">
         <f t="shared" si="5"/>
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="L48">
         <v>7289800</v>
@@ -4073,30 +4079,30 @@
       </c>
       <c r="P48">
         <f t="shared" si="8"/>
-        <v>37</v>
+        <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>63</v>
       </c>
-      <c r="B49" s="12">
+      <c r="B49">
         <v>92200</v>
       </c>
-      <c r="C49" s="12">
+      <c r="C49">
         <v>90499.43</v>
       </c>
-      <c r="D49" s="12">
+      <c r="D49">
         <f t="shared" si="0"/>
         <v>-1700.570000000007</v>
       </c>
-      <c r="E49" s="13">
+      <c r="E49" s="5">
         <f t="shared" si="1"/>
         <v>-1.8444360086767971E-2</v>
       </c>
-      <c r="F49" s="12">
+      <c r="F49">
         <f t="shared" si="2"/>
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G49">
         <v>102600</v>
@@ -4114,7 +4120,7 @@
       </c>
       <c r="K49">
         <f t="shared" si="5"/>
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="L49">
         <v>0</v>
@@ -4130,32 +4136,32 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="P49">
+      <c r="P49" t="str">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>64</v>
       </c>
-      <c r="B50" s="12">
+      <c r="B50">
         <v>832600</v>
       </c>
-      <c r="C50" s="12">
+      <c r="C50">
         <v>832600</v>
       </c>
-      <c r="D50" s="12">
+      <c r="D50">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E50" s="13">
+      <c r="E50" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F50" s="12">
+      <c r="F50" t="str">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v/>
       </c>
       <c r="G50">
         <v>859100</v>
@@ -4171,9 +4177,9 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K50">
+      <c r="K50" t="str">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v/>
       </c>
       <c r="L50">
         <v>843200</v>
@@ -4189,32 +4195,32 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="P50">
+      <c r="P50" t="str">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>65</v>
       </c>
-      <c r="B51" s="12">
+      <c r="B51">
         <v>8609500</v>
       </c>
-      <c r="C51" s="12">
+      <c r="C51">
         <v>8499425.3399999905</v>
       </c>
-      <c r="D51" s="12">
+      <c r="D51">
         <f t="shared" si="0"/>
         <v>-110074.66000000946</v>
       </c>
-      <c r="E51" s="13">
+      <c r="E51" s="5">
         <f t="shared" si="1"/>
         <v>-1.2785255822058129E-2</v>
       </c>
-      <c r="F51" s="12">
+      <c r="F51">
         <f t="shared" si="2"/>
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="G51">
         <v>8925500</v>
@@ -4232,7 +4238,7 @@
       </c>
       <c r="K51">
         <f t="shared" si="5"/>
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="L51">
         <v>8833900</v>
@@ -4250,30 +4256,30 @@
       </c>
       <c r="P51">
         <f t="shared" si="8"/>
-        <v>19</v>
+        <v>33</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>66</v>
       </c>
-      <c r="B52" s="12">
+      <c r="B52">
         <v>2451000</v>
       </c>
-      <c r="C52" s="12">
+      <c r="C52">
         <v>2254684.7999999998</v>
       </c>
-      <c r="D52" s="12">
+      <c r="D52">
         <f t="shared" si="0"/>
         <v>-196315.20000000019</v>
       </c>
-      <c r="E52" s="13">
+      <c r="E52" s="5">
         <f t="shared" si="1"/>
         <v>-8.009596083231342E-2</v>
       </c>
-      <c r="F52" s="12">
+      <c r="F52">
         <f t="shared" si="2"/>
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="G52">
         <v>2440700</v>
@@ -4291,7 +4297,7 @@
       </c>
       <c r="K52">
         <f t="shared" si="5"/>
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="L52">
         <v>2321600</v>
@@ -4309,15 +4315,15 @@
       </c>
       <c r="P52">
         <f t="shared" si="8"/>
-        <v>46</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A54" s="2" t="s">
-        <v>67</v>
+      <c r="A54" s="11" t="s">
+        <v>87</v>
       </c>
       <c r="F54" s="11" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.2">
@@ -4540,9 +4546,11 @@
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A63" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="F63" s="7"/>
+        <v>88</v>
+      </c>
+      <c r="F63" s="7" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
@@ -4589,16 +4597,16 @@
       <c r="F65" t="s">
         <v>24</v>
       </c>
-      <c r="G65" t="e">
-        <f>_xlfn.XLOOKUP(F65,$A$2:$A$52,MATCH(G64,$A$1:$P$1,0))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H65">
-        <f>_xlfn.XLOOKUP(F65,$A$2:$A$52,$I$2:$I$52)</f>
+      <c r="G65" cm="1">
+        <f t="array" ref="G65">_xlfn.XLOOKUP($F65,$A$2:$A$52,_xlfn.XLOOKUP(G$64,$A$1:$P$1,$A$2:$P$52))</f>
+        <v>-36209.630000000005</v>
+      </c>
+      <c r="H65" cm="1">
+        <f t="array" ref="H65">_xlfn.XLOOKUP($F65,$A$2:$A$52,_xlfn.XLOOKUP(H$64,$A$1:$P$1,$A$2:$P$52))</f>
         <v>-27292.159999999974</v>
       </c>
-      <c r="I65">
-        <f>_xlfn.XLOOKUP(F65,$A$2:$A$52,$N$2:$N$52)</f>
+      <c r="I65" cm="1">
+        <f t="array" ref="I65">_xlfn.XLOOKUP($F65,$A$2:$A$52,_xlfn.XLOOKUP(I$64,$A$1:$P$1,$A$2:$P$52))</f>
         <v>-9181.0800000000163</v>
       </c>
     </row>
@@ -4621,16 +4629,16 @@
       <c r="F66" t="s">
         <v>25</v>
       </c>
-      <c r="G66">
-        <f>_xlfn.XLOOKUP(F66,$A$2:$A$52,$D$2:$D$52)</f>
-        <v>0</v>
-      </c>
-      <c r="H66">
-        <f t="shared" ref="H66:H70" si="14">_xlfn.XLOOKUP(F66,$A$2:$A$52,$I$2:$I$52)</f>
-        <v>0</v>
-      </c>
-      <c r="I66">
-        <f t="shared" ref="I66:I70" si="15">_xlfn.XLOOKUP(F66,$A$2:$A$52,$N$2:$N$52)</f>
+      <c r="G66" cm="1">
+        <f t="array" ref="G66">_xlfn.XLOOKUP($F66,$A$2:$A$52,_xlfn.XLOOKUP(G$64,$A$1:$P$1,$A$2:$P$52))</f>
+        <v>0</v>
+      </c>
+      <c r="H66" cm="1">
+        <f t="array" ref="H66">_xlfn.XLOOKUP($F66,$A$2:$A$52,_xlfn.XLOOKUP(H$64,$A$1:$P$1,$A$2:$P$52))</f>
+        <v>0</v>
+      </c>
+      <c r="I66" cm="1">
+        <f t="array" ref="I66">_xlfn.XLOOKUP($F66,$A$2:$A$52,_xlfn.XLOOKUP(I$64,$A$1:$P$1,$A$2:$P$52))</f>
         <v>-311228.08999999997</v>
       </c>
     </row>
@@ -4653,16 +4661,16 @@
       <c r="F67" t="s">
         <v>32</v>
       </c>
-      <c r="G67">
-        <f t="shared" ref="G66:G70" si="16">_xlfn.XLOOKUP(F67,$A$2:$A$52,$D$2:$D$52)</f>
+      <c r="G67" cm="1">
+        <f t="array" ref="G67">_xlfn.XLOOKUP($F67,$A$2:$A$52,_xlfn.XLOOKUP(G$64,$A$1:$P$1,$A$2:$P$52))</f>
         <v>-149396.10000000987</v>
       </c>
-      <c r="H67">
-        <f t="shared" si="14"/>
+      <c r="H67" cm="1">
+        <f t="array" ref="H67">_xlfn.XLOOKUP($F67,$A$2:$A$52,_xlfn.XLOOKUP(H$64,$A$1:$P$1,$A$2:$P$52))</f>
         <v>-189254.06000000006</v>
       </c>
-      <c r="I67">
-        <f t="shared" si="15"/>
+      <c r="I67" cm="1">
+        <f t="array" ref="I67">_xlfn.XLOOKUP($F67,$A$2:$A$52,_xlfn.XLOOKUP(I$64,$A$1:$P$1,$A$2:$P$52))</f>
         <v>-374962.91000000015</v>
       </c>
     </row>
@@ -4685,16 +4693,16 @@
       <c r="F68" t="s">
         <v>38</v>
       </c>
-      <c r="G68">
-        <f t="shared" si="16"/>
+      <c r="G68" cm="1">
+        <f t="array" ref="G68">_xlfn.XLOOKUP($F68,$A$2:$A$52,_xlfn.XLOOKUP(G$64,$A$1:$P$1,$A$2:$P$52))</f>
         <v>-12230.810000000056</v>
       </c>
-      <c r="H68">
-        <f t="shared" si="14"/>
+      <c r="H68" cm="1">
+        <f t="array" ref="H68">_xlfn.XLOOKUP($F68,$A$2:$A$52,_xlfn.XLOOKUP(H$64,$A$1:$P$1,$A$2:$P$52))</f>
         <v>-45485.580000000075</v>
       </c>
-      <c r="I68">
-        <f t="shared" si="15"/>
+      <c r="I68" cm="1">
+        <f t="array" ref="I68">_xlfn.XLOOKUP($F68,$A$2:$A$52,_xlfn.XLOOKUP(I$64,$A$1:$P$1,$A$2:$P$52))</f>
         <v>-72.879999999888241</v>
       </c>
     </row>
@@ -4717,16 +4725,16 @@
       <c r="F69" t="s">
         <v>39</v>
       </c>
-      <c r="G69">
-        <f t="shared" si="16"/>
+      <c r="G69" cm="1">
+        <f t="array" ref="G69">_xlfn.XLOOKUP($F69,$A$2:$A$52,_xlfn.XLOOKUP(G$64,$A$1:$P$1,$A$2:$P$52))</f>
         <v>-4950.4699999999721</v>
       </c>
-      <c r="H69">
-        <f t="shared" si="14"/>
+      <c r="H69" cm="1">
+        <f t="array" ref="H69">_xlfn.XLOOKUP($F69,$A$2:$A$52,_xlfn.XLOOKUP(H$64,$A$1:$P$1,$A$2:$P$52))</f>
         <v>-8005.7900000010268</v>
       </c>
-      <c r="I69">
-        <f t="shared" si="15"/>
+      <c r="I69" cm="1">
+        <f t="array" ref="I69">_xlfn.XLOOKUP($F69,$A$2:$A$52,_xlfn.XLOOKUP(I$64,$A$1:$P$1,$A$2:$P$52))</f>
         <v>-1724.9000000000233</v>
       </c>
     </row>
@@ -4749,24 +4757,26 @@
       <c r="F70" t="s">
         <v>55</v>
       </c>
-      <c r="G70">
-        <f t="shared" si="16"/>
+      <c r="G70" cm="1">
+        <f t="array" ref="G70">_xlfn.XLOOKUP($F70,$A$2:$A$52,_xlfn.XLOOKUP(G$64,$A$1:$P$1,$A$2:$P$52))</f>
         <v>-184239.79000001028</v>
       </c>
-      <c r="H70">
-        <f t="shared" si="14"/>
+      <c r="H70" cm="1">
+        <f t="array" ref="H70">_xlfn.XLOOKUP($F70,$A$2:$A$52,_xlfn.XLOOKUP(H$64,$A$1:$P$1,$A$2:$P$52))</f>
         <v>-133456.33000001032</v>
       </c>
-      <c r="I70">
-        <f t="shared" si="15"/>
+      <c r="I70" cm="1">
+        <f t="array" ref="I70">_xlfn.XLOOKUP($F70,$A$2:$A$52,_xlfn.XLOOKUP(I$64,$A$1:$P$1,$A$2:$P$52))</f>
         <v>-82077.349999999627</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F72" s="7"/>
+        <v>89</v>
+      </c>
+      <c r="F72" s="7" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
@@ -4813,16 +4823,16 @@
       <c r="F74" t="s">
         <v>24</v>
       </c>
-      <c r="G74" t="e">
-        <f>INDEX($D$2:$D$52,MATCH(F74,$A$2:$A$52,0),MATCH(G73,$A$1:$P$1,0))</f>
-        <v>#REF!</v>
+      <c r="G74">
+        <f>INDEX($A$2:$P$52,MATCH($F74,$A$2:$A$52,0),MATCH(G$73,$A$1:$P$1,0))</f>
+        <v>-36209.630000000005</v>
       </c>
       <c r="H74">
-        <f>INDEX($I$2:$I$52,MATCH(F74,$A$2:$A$52,0))</f>
+        <f>INDEX($A$2:$P$52,MATCH($F74,$A$2:$A$52,0),MATCH(H$73,$A$1:$P$1,0))</f>
         <v>-27292.159999999974</v>
       </c>
       <c r="I74">
-        <f>INDEX($N$2:$N$52,MATCH(F74,$A$2:$A$52,0))</f>
+        <f>INDEX($A$2:$P$52,MATCH($F74,$A$2:$A$52,0),MATCH(I$73,$A$1:$P$1,0))</f>
         <v>-9181.0800000000163</v>
       </c>
     </row>
@@ -4831,30 +4841,30 @@
         <v>25</v>
       </c>
       <c r="B75">
-        <f t="shared" ref="B75:B79" si="17">INDEX($D$2:$D$52,MATCH(A75,$A$2:$A$52,0))</f>
+        <f t="shared" ref="B75:B79" si="14">INDEX($D$2:$D$52,MATCH(A75,$A$2:$A$52,0))</f>
         <v>0</v>
       </c>
       <c r="C75">
-        <f t="shared" ref="C75:C79" si="18">INDEX($I$2:$I$52,MATCH(A75,$A$2:$A$52,0))</f>
+        <f t="shared" ref="C75:C79" si="15">INDEX($I$2:$I$52,MATCH(A75,$A$2:$A$52,0))</f>
         <v>0</v>
       </c>
       <c r="D75">
-        <f t="shared" ref="D75:D79" si="19">INDEX($N$2:$N$52,MATCH(A75,$A$2:$A$52,0))</f>
+        <f t="shared" ref="D75:D79" si="16">INDEX($N$2:$N$52,MATCH(A75,$A$2:$A$52,0))</f>
         <v>-311228.08999999997</v>
       </c>
       <c r="F75" t="s">
         <v>25</v>
       </c>
       <c r="G75">
-        <f t="shared" ref="G75:G79" si="20">INDEX($D$2:$D$52,MATCH(F75,$A$2:$A$52,0))</f>
+        <f t="shared" ref="G75:I79" si="17">INDEX($A$2:$P$52,MATCH($F75,$A$2:$A$52,0),MATCH(G$73,$A$1:$P$1,0))</f>
         <v>0</v>
       </c>
       <c r="H75">
-        <f t="shared" ref="H75:H79" si="21">INDEX($I$2:$I$52,MATCH(F75,$A$2:$A$52,0))</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="I75">
-        <f t="shared" ref="I75:I79" si="22">INDEX($N$2:$N$52,MATCH(F75,$A$2:$A$52,0))</f>
+        <f t="shared" si="17"/>
         <v>-311228.08999999997</v>
       </c>
     </row>
@@ -4863,30 +4873,30 @@
         <v>32</v>
       </c>
       <c r="B76">
+        <f t="shared" si="14"/>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="15"/>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="16"/>
+        <v>-374962.91000000015</v>
+      </c>
+      <c r="F76" t="s">
+        <v>32</v>
+      </c>
+      <c r="G76">
         <f t="shared" si="17"/>
         <v>-149396.10000000987</v>
       </c>
-      <c r="C76">
-        <f t="shared" si="18"/>
+      <c r="H76">
+        <f t="shared" si="17"/>
         <v>-189254.06000000006</v>
       </c>
-      <c r="D76">
-        <f t="shared" si="19"/>
-        <v>-374962.91000000015</v>
-      </c>
-      <c r="F76" t="s">
-        <v>32</v>
-      </c>
-      <c r="G76">
-        <f t="shared" si="20"/>
-        <v>-149396.10000000987</v>
-      </c>
-      <c r="H76">
-        <f t="shared" si="21"/>
-        <v>-189254.06000000006</v>
-      </c>
       <c r="I76">
-        <f t="shared" si="22"/>
+        <f t="shared" si="17"/>
         <v>-374962.91000000015</v>
       </c>
     </row>
@@ -4895,30 +4905,30 @@
         <v>38</v>
       </c>
       <c r="B77">
+        <f t="shared" si="14"/>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="C77">
+        <f t="shared" si="15"/>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="16"/>
+        <v>-72.879999999888241</v>
+      </c>
+      <c r="F77" t="s">
+        <v>38</v>
+      </c>
+      <c r="G77">
         <f t="shared" si="17"/>
         <v>-12230.810000000056</v>
       </c>
-      <c r="C77">
-        <f t="shared" si="18"/>
+      <c r="H77">
+        <f t="shared" si="17"/>
         <v>-45485.580000000075</v>
       </c>
-      <c r="D77">
-        <f t="shared" si="19"/>
-        <v>-72.879999999888241</v>
-      </c>
-      <c r="F77" t="s">
-        <v>38</v>
-      </c>
-      <c r="G77">
-        <f t="shared" si="20"/>
-        <v>-12230.810000000056</v>
-      </c>
-      <c r="H77">
-        <f t="shared" si="21"/>
-        <v>-45485.580000000075</v>
-      </c>
       <c r="I77">
-        <f t="shared" si="22"/>
+        <f t="shared" si="17"/>
         <v>-72.879999999888241</v>
       </c>
     </row>
@@ -4927,30 +4937,30 @@
         <v>39</v>
       </c>
       <c r="B78">
+        <f t="shared" si="14"/>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="C78">
+        <f t="shared" si="15"/>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="16"/>
+        <v>-1724.9000000000233</v>
+      </c>
+      <c r="F78" t="s">
+        <v>39</v>
+      </c>
+      <c r="G78">
         <f t="shared" si="17"/>
         <v>-4950.4699999999721</v>
       </c>
-      <c r="C78">
-        <f t="shared" si="18"/>
+      <c r="H78">
+        <f t="shared" si="17"/>
         <v>-8005.7900000010268</v>
       </c>
-      <c r="D78">
-        <f t="shared" si="19"/>
-        <v>-1724.9000000000233</v>
-      </c>
-      <c r="F78" t="s">
-        <v>39</v>
-      </c>
-      <c r="G78">
-        <f t="shared" si="20"/>
-        <v>-4950.4699999999721</v>
-      </c>
-      <c r="H78">
-        <f t="shared" si="21"/>
-        <v>-8005.7900000010268</v>
-      </c>
       <c r="I78">
-        <f t="shared" si="22"/>
+        <f t="shared" si="17"/>
         <v>-1724.9000000000233</v>
       </c>
     </row>
@@ -4959,36 +4969,36 @@
         <v>55</v>
       </c>
       <c r="B79">
+        <f t="shared" si="14"/>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="C79">
+        <f t="shared" si="15"/>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="D79">
+        <f t="shared" si="16"/>
+        <v>-82077.349999999627</v>
+      </c>
+      <c r="F79" t="s">
+        <v>55</v>
+      </c>
+      <c r="G79">
         <f t="shared" si="17"/>
         <v>-184239.79000001028</v>
       </c>
-      <c r="C79">
-        <f t="shared" si="18"/>
+      <c r="H79">
+        <f t="shared" si="17"/>
         <v>-133456.33000001032</v>
       </c>
-      <c r="D79">
-        <f t="shared" si="19"/>
-        <v>-82077.349999999627</v>
-      </c>
-      <c r="F79" t="s">
-        <v>55</v>
-      </c>
-      <c r="G79">
-        <f t="shared" si="20"/>
-        <v>-184239.79000001028</v>
-      </c>
-      <c r="H79">
-        <f t="shared" si="21"/>
-        <v>-133456.33000001032</v>
-      </c>
       <c r="I79">
-        <f t="shared" si="22"/>
+        <f t="shared" si="17"/>
         <v>-82077.349999999627</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
@@ -5001,15 +5011,15 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B83" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B84" s="6">
         <f>INDEX($B$2:$B$52,MATCH(B82,$A$2:$A$52,0))</f>
@@ -5022,7 +5032,7 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B85" s="6">
         <f>INDEX($G$2:$G$52,MATCH(B82,$A$2:$A$52,0))</f>
@@ -5035,7 +5045,7 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B86" s="6">
         <f>INDEX($L$2:$L$52,MATCH(B82,$A$2:$A$52,0))</f>
@@ -5048,12 +5058,12 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B89" s="7">
         <v>1</v>
@@ -5072,53 +5082,116 @@
         <v>0</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D90" s="8" t="s">
         <v>0</v>
       </c>
       <c r="E90" s="8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F90" s="8" t="s">
         <v>0</v>
       </c>
       <c r="G90" s="8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>73</v>
-      </c>
-      <c r="C91" s="5"/>
-      <c r="E91" s="5"/>
-      <c r="G91" s="5"/>
+        <v>70</v>
+      </c>
+      <c r="B91" t="str">
+        <f>_xlfn.XLOOKUP($B$89,$F$2:$F$52,$A$2:$A$52)</f>
+        <v>Clerk and Master - Chancery</v>
+      </c>
+      <c r="C91" s="5">
+        <f>_xlfn.XLOOKUP(B91,$A$2:$A$52,$E$2:$E$52)</f>
+        <v>-0.15235918433091292</v>
+      </c>
+      <c r="D91" t="str">
+        <f>_xlfn.XLOOKUP($D$89,$F$2:$F$52,$A$2:$A$52)</f>
+        <v>Circuit Court Clerk</v>
+      </c>
+      <c r="E91" s="5">
+        <f>_xlfn.XLOOKUP(D91,$A$2:$A$52,$E$2:$E$52)</f>
+        <v>-0.11502817362571344</v>
+      </c>
+      <c r="F91" t="str">
+        <f>_xlfn.XLOOKUP($F$89,$F$2:$F$52,$A$2:$A$52)</f>
+        <v>Internal Audit</v>
+      </c>
+      <c r="G91" s="5">
+        <f>_xlfn.XLOOKUP(F91,$A$2:$A$52,$E$2:$E$52)</f>
+        <v>-9.5782760864849215E-2</v>
+      </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>74</v>
-      </c>
-      <c r="C92" s="5"/>
-      <c r="E92" s="5"/>
-      <c r="G92" s="5"/>
+        <v>71</v>
+      </c>
+      <c r="B92" t="str">
+        <f>_xlfn.XLOOKUP($B$89,$K$2:$K$52,$A$2:$A$52)</f>
+        <v>Metropolitan Clerk</v>
+      </c>
+      <c r="C92" s="5">
+        <f>_xlfn.XLOOKUP(B92,$A$2:$A$52,$J$2:$J$52)</f>
+        <v>-0.17551246244575608</v>
+      </c>
+      <c r="D92" t="str">
+        <f>_xlfn.XLOOKUP($D$89,$K$2:$K$52,$A$2:$A$52)</f>
+        <v>Internal Audit</v>
+      </c>
+      <c r="E92" s="5">
+        <f>_xlfn.XLOOKUP(D92,$A$2:$A$52,$J$2:$J$52)</f>
+        <v>-0.17103239309050916</v>
+      </c>
+      <c r="F92" t="str">
+        <f>_xlfn.XLOOKUP($F$89,$K$2:$K$52,$A$2:$A$52)</f>
+        <v>Office of Family Safety</v>
+      </c>
+      <c r="G92" s="5">
+        <f>_xlfn.XLOOKUP(F92,$A$2:$A$52,$J$2:$J$52)</f>
+        <v>-0.13918241656366656</v>
+      </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>75</v>
-      </c>
-      <c r="C93" s="5"/>
-      <c r="E93" s="5"/>
-      <c r="G93" s="5"/>
+        <v>72</v>
+      </c>
+      <c r="B93" t="str">
+        <f>_xlfn.XLOOKUP($B$89,$P$2:$P$52,$A$2:$A$52)</f>
+        <v>Community Oversight Board</v>
+      </c>
+      <c r="C93" s="5">
+        <f>_xlfn.XLOOKUP(B93,$A$2:$A$52,$O$2:$O$52)</f>
+        <v>-0.82994157333333329</v>
+      </c>
+      <c r="D93" t="str">
+        <f>_xlfn.XLOOKUP($D$89,$P$2:$P$52,$A$2:$A$52)</f>
+        <v>Clerk and Master - Chancery</v>
+      </c>
+      <c r="E93" s="5">
+        <f>_xlfn.XLOOKUP(D93,$A$2:$A$52,$O$2:$O$52)</f>
+        <v>-0.15295680364719175</v>
+      </c>
+      <c r="F93" t="str">
+        <f>_xlfn.XLOOKUP($F$89,$P$2:$P$52,$A$2:$A$52)</f>
+        <v>Election Commission</v>
+      </c>
+      <c r="G93" s="5">
+        <f>_xlfn.XLOOKUP(F93,$A$2:$A$52,$O$2:$O$52)</f>
+        <v>-0.12882667147667154</v>
+      </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B96" s="7">
         <v>1</v>
@@ -5137,47 +5210,119 @@
         <v>0</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D97" s="8" t="s">
         <v>0</v>
       </c>
       <c r="E97" s="8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F97" s="8" t="s">
         <v>0</v>
       </c>
       <c r="G97" s="8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>73</v>
-      </c>
-      <c r="C98" s="4"/>
-      <c r="E98" s="4"/>
-      <c r="G98" s="4"/>
+        <v>70</v>
+      </c>
+      <c r="B98" t="str">
+        <f>INDEX($A$2:$A$52,MATCH($B$96,$F$2:$F$52,0))</f>
+        <v>Clerk and Master - Chancery</v>
+      </c>
+      <c r="C98" s="4">
+        <f>INDEX($E$2:$E$52,MATCH(B98,$A$2:$A$52,0))</f>
+        <v>-0.15235918433091292</v>
+      </c>
+      <c r="D98" t="str">
+        <f>INDEX($A$2:$A$52,MATCH($D$96,$F$2:$F$52,0))</f>
+        <v>Circuit Court Clerk</v>
+      </c>
+      <c r="E98" s="4">
+        <f>INDEX($E$2:$E$52,MATCH(D98,$A$2:$A$52,0))</f>
+        <v>-0.11502817362571344</v>
+      </c>
+      <c r="F98" t="str">
+        <f>INDEX($A$2:$A$52,MATCH($F$96,$F$2:$F$52,0))</f>
+        <v>Internal Audit</v>
+      </c>
+      <c r="G98" s="4">
+        <f>INDEX($E$2:$E$52,MATCH(F98,$A$2:$A$52,0))</f>
+        <v>-9.5782760864849215E-2</v>
+      </c>
       <c r="I98" s="4"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>74</v>
-      </c>
-      <c r="C99" s="4"/>
-      <c r="E99" s="4"/>
-      <c r="G99" s="4"/>
+        <v>71</v>
+      </c>
+      <c r="B99" t="str">
+        <f>INDEX($A$2:$A$52,MATCH($B$96,$K$2:$K$52,0))</f>
+        <v>Metropolitan Clerk</v>
+      </c>
+      <c r="C99" s="4">
+        <f>INDEX($J$2:$J$52,MATCH(B99,$A$2:$A$52,0))</f>
+        <v>-0.17551246244575608</v>
+      </c>
+      <c r="D99" t="str">
+        <f>INDEX($A$2:$A$52,MATCH($D$96,$K$2:$K$52,0))</f>
+        <v>Internal Audit</v>
+      </c>
+      <c r="E99" s="4">
+        <f>INDEX($J$2:$J$52,MATCH(D99,$A$2:$A$52,0))</f>
+        <v>-0.17103239309050916</v>
+      </c>
+      <c r="F99" t="str">
+        <f>INDEX($A$2:$A$52,MATCH($F$96,$K$2:$K$52,0))</f>
+        <v>Office of Family Safety</v>
+      </c>
+      <c r="G99" s="4">
+        <f>INDEX($J$2:$J$52,MATCH(F99,$A$2:$A$52,0))</f>
+        <v>-0.13918241656366656</v>
+      </c>
       <c r="I99" s="4"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>75</v>
-      </c>
-      <c r="C100" s="4"/>
-      <c r="E100" s="4"/>
-      <c r="G100" s="4"/>
+        <v>72</v>
+      </c>
+      <c r="B100" t="str">
+        <f>INDEX($A$2:$A$52,MATCH($B$96,$P$2:$P$52,0))</f>
+        <v>Community Oversight Board</v>
+      </c>
+      <c r="C100" s="4">
+        <f>INDEX($O$2:$O$52,MATCH(B100,$A$2:$A$52,0))</f>
+        <v>-0.82994157333333329</v>
+      </c>
+      <c r="D100" t="str">
+        <f>INDEX($A$2:$A$52,MATCH($D$96,$P$2:$P$52,0))</f>
+        <v>Clerk and Master - Chancery</v>
+      </c>
+      <c r="E100" s="4">
+        <f>INDEX($O$2:$O$52,MATCH(D100,$A$2:$A$52,0))</f>
+        <v>-0.15295680364719175</v>
+      </c>
+      <c r="F100" t="str">
+        <f>INDEX($A$2:$A$52,MATCH($F$96,$P$2:$P$52,0))</f>
+        <v>Election Commission</v>
+      </c>
+      <c r="G100" s="4">
+        <f>INDEX($O$2:$O$52,MATCH(F100,$A$2:$A$52,0))</f>
+        <v>-0.12882667147667154</v>
+      </c>
       <c r="I100" s="4"/>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D105" s="5"/>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D106" s="5"/>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D107" s="5"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -5209,7 +5354,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -5217,7 +5362,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -5225,7 +5370,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -5233,7 +5378,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -5241,7 +5386,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -5249,7 +5394,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -5257,7 +5402,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -5265,7 +5410,7 @@
         <v>11</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -5273,7 +5418,7 @@
         <v>12</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -5281,7 +5426,7 @@
         <v>13</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
metro budget exercises with bar chart
</commit_message>
<xml_diff>
--- a/spreadsheets/metro_budget_exercise.xlsx
+++ b/spreadsheets/metro_budget_exercise.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aimeejohnson/Desktop/DA12/projects/excel-lookups-da12-aimeejohnson/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04AE6114-9129-BD44-B833-5ADC6572A845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F34311-6ED7-D341-AF5A-8A7A5B920123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4980" windowWidth="33600" windowHeight="19080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38320" windowHeight="20440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metro_budget" sheetId="1" r:id="rId1"/>
@@ -942,6 +942,999 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Department Budget</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>metro_budget!$B$83</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Budget</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>metro_budget!$A$84:$A$86</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>FY17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FY18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FY19</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>metro_budget!$B$84:$B$86</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>356640100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>382685200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>376548600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C26F-ED42-89DC-F1FE5C8CC799}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>metro_budget!$C$83</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>metro_budget!$A$84:$A$86</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>FY17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FY18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FY19</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>metro_budget!$C$84:$C$86</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>341243679.13</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>346340810.81999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>355279492.22999901</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C26F-ED42-89DC-F1FE5C8CC799}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="946451904"/>
+        <c:axId val="946453616"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="946451904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="946453616"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="946453616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="946451904"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>517153</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>52860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>684198</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>72997</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF3DF943-B6BF-C4CB-7AA7-CD24A9F00EF4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
@@ -1241,8 +2234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P107"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
-      <selection activeCell="G100" sqref="G100"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="111" workbookViewId="0">
+      <selection activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5332,6 +6325,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B83" xr:uid="{1248789C-8354-428B-8B98-C97B02054C67}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>